<commit_message>
Risolto tutto, ma rimane un problema abbastanza grosso nel calcolo di setup di LS2: tutti gli altri valori sono computati correttamenti, non funziona solo quello
</commit_message>
<xml_diff>
--- a/PS-VRP/Dati_output/insert_inter.xlsx
+++ b/PS-VRP/Dati_output/insert_inter.xlsx
@@ -416,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T27"/>
+  <dimension ref="A1:S27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -515,41 +515,41 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>251651</v>
+        <v>250759</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>BIMEC 4</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="D2" t="n">
-        <v>767.7049180327868</v>
+        <v>118.2816901408451</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2025-05-09 07:00:00</t>
+          <t>2025-05-08 07:00:00</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2025-05-09 07:29:00</t>
+          <t>2025-05-08 07:19:00</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>2025-05-09 07:29:00</t>
+          <t>2025-05-08 07:19:00</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>2025-05-12 12:16:42</t>
+          <t>2025-05-08 09:17:16</t>
         </is>
       </c>
       <c r="I2" t="n">
-        <v>46830</v>
+        <v>8398</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
@@ -558,95 +558,96 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12</t>
         </is>
       </c>
       <c r="L2" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M2" t="n">
         <v>76</v>
       </c>
       <c r="N2" t="n">
-        <v>39755</v>
-      </c>
-      <c r="O2" t="n">
-        <v>0</v>
+        <v>39747</v>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
       </c>
       <c r="P2" t="n">
-        <v>0</v>
+        <v>39747</v>
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>2025-05-12 00:00:00</t>
+          <t>2025-03-13 00:00:00</t>
         </is>
       </c>
       <c r="R2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="S2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="T2" t="n">
-        <v>4</v>
+        <v>-0.3870011737037037</v>
+      </c>
+      <c r="S2" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>251391</v>
+        <v>251706</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>T3</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>96.14754098360656</v>
+        <v>50.79365079365079</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2025-05-08 07:00:00</t>
+          <t>2025-05-12 07:00:00</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2025-05-08 07:35:00</t>
+          <t>2025-05-12 07:00:00</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>2025-05-08 07:35:00</t>
+          <t>2025-05-12 07:00:00</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>2025-05-08 09:11:08</t>
+          <t>2025-05-12 07:50:47</t>
         </is>
       </c>
       <c r="I3" t="n">
-        <v>5865</v>
+        <v>3200</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>bobina</t>
+          <t>foglio</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>T3</t>
         </is>
       </c>
       <c r="L3" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="M3" t="n">
-        <v>70</v>
-      </c>
-      <c r="N3" t="n">
-        <v>39749</v>
+        <v>0</v>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>39764 (esterno)</t>
+        </is>
       </c>
       <c r="O3" t="inlineStr">
         <is>
@@ -654,60 +655,57 @@
         </is>
       </c>
       <c r="P3" t="n">
-        <v>39749</v>
+        <v>39764</v>
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>2025-04-23 00:00:00</t>
+          <t>2025-05-14 00:00:00</t>
         </is>
       </c>
       <c r="R3" s="1" t="n">
-        <v>-0.4377821180555556</v>
-      </c>
-      <c r="S3" s="1" t="n">
-        <v>-1.382741347905093</v>
-      </c>
-      <c r="T3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S3" t="n">
         <v>7</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>251840</v>
+        <v>251164</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>20</v>
+        <v>57</v>
       </c>
       <c r="D4" t="n">
-        <v>93.67213114754098</v>
+        <v>140.8450704225352</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2025-05-08 09:11:08</t>
+          <t>2025-05-09 07:00:00</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>2025-05-08 09:31:08</t>
+          <t>2025-05-09 07:57:00</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>2025-05-08 09:31:08</t>
+          <t>2025-05-09 07:57:00</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>2025-05-08 11:04:49</t>
+          <t>2025-05-09 10:17:50</t>
         </is>
       </c>
       <c r="I4" t="n">
-        <v>5714</v>
+        <v>10000</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
@@ -720,13 +718,13 @@
         </is>
       </c>
       <c r="L4" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M4" t="n">
         <v>70</v>
       </c>
       <c r="N4" t="n">
-        <v>39758</v>
+        <v>39749</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
@@ -734,60 +732,57 @@
         </is>
       </c>
       <c r="P4" t="n">
-        <v>39758</v>
+        <v>39749</v>
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>2025-05-09 00:00:00</t>
+          <t>2025-04-22 00:00:00</t>
         </is>
       </c>
       <c r="R4" s="1" t="n">
-        <v>-0.4885587431712963</v>
-      </c>
-      <c r="S4" s="1" t="n">
-        <v>-0.4616803278703704</v>
-      </c>
-      <c r="T4" t="n">
-        <v>1</v>
+        <v>-2.429059076678241</v>
+      </c>
+      <c r="S4" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>251742</v>
+        <v>251050</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>25</v>
+        <v>195</v>
       </c>
       <c r="D5" t="n">
-        <v>134.8524590163935</v>
+        <v>0</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2025-05-08 11:04:49</t>
+          <t>2025-05-09 10:17:50</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>2025-05-08 11:29:49</t>
+          <t>2025-05-09 13:32:50</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>2025-05-08 11:29:49</t>
+          <t>2025-05-09 13:32:50</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>2025-05-08 13:44:40</t>
+          <t>2025-05-09 13:32:50</t>
         </is>
       </c>
       <c r="I5" t="n">
-        <v>8226</v>
+        <v>0</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
@@ -796,17 +791,17 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="L5" t="n">
-        <v>4</v>
+        <v>38</v>
       </c>
       <c r="M5" t="n">
         <v>70</v>
       </c>
       <c r="N5" t="n">
-        <v>39749</v>
+        <v>39747</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
@@ -814,60 +809,57 @@
         </is>
       </c>
       <c r="P5" t="n">
-        <v>39749</v>
+        <v>39747</v>
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>2025-05-15 00:00:00</t>
+          <t>2025-04-16 00:00:00</t>
         </is>
       </c>
       <c r="R5" s="1" t="n">
-        <v>-1.406147540983796</v>
-      </c>
-      <c r="S5" s="1" t="n">
-        <v>-1.572688979965278</v>
-      </c>
-      <c r="T5" t="n">
-        <v>7</v>
+        <v>-1.564475743344907</v>
+      </c>
+      <c r="S5" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>251229</v>
+        <v>251054</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D6" t="n">
-        <v>307.1967213114754</v>
+        <v>0</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2025-05-08 13:44:40</t>
+          <t>2025-05-09 13:32:50</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2025-05-08 14:14:40</t>
+          <t>2025-05-09 14:07:50</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>2025-05-08 14:14:40</t>
+          <t>2025-05-09 14:07:50</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>2025-05-09 11:21:52</t>
+          <t>2025-05-09 14:07:50</t>
         </is>
       </c>
       <c r="I6" t="n">
-        <v>18739</v>
+        <v>0</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
@@ -876,19 +868,17 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R9</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="L6" t="n">
-        <v>6</v>
+        <v>38</v>
       </c>
       <c r="M6" t="n">
         <v>70</v>
       </c>
-      <c r="N6" t="inlineStr">
-        <is>
-          <t>39723 (esterno)</t>
-        </is>
+      <c r="N6" t="n">
+        <v>39747</v>
       </c>
       <c r="O6" t="inlineStr">
         <is>
@@ -896,60 +886,57 @@
         </is>
       </c>
       <c r="P6" t="n">
-        <v>39723</v>
+        <v>39747</v>
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>2025-05-15 00:00:00</t>
+          <t>2025-04-16 00:00:00</t>
         </is>
       </c>
       <c r="R6" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="S6" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="T6" t="n">
-        <v>1</v>
+        <v>-1.588781298900463</v>
+      </c>
+      <c r="S6" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>251164</v>
+        <v>251081</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>23</v>
+        <v>125</v>
       </c>
       <c r="D7" t="n">
-        <v>156.25</v>
+        <v>42.42253521126761</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2025-05-07 07:00:00</t>
+          <t>2025-05-09 14:07:50</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>2025-05-07 07:23:00</t>
+          <t>2025-05-12 08:12:50</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>2025-05-07 07:23:00</t>
+          <t>2025-05-12 08:12:50</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>2025-05-07 09:59:15</t>
+          <t>2025-05-12 08:55:16</t>
         </is>
       </c>
       <c r="I7" t="n">
-        <v>10000</v>
+        <v>3012</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
@@ -958,17 +945,19 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="L7" t="n">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="M7" t="n">
         <v>70</v>
       </c>
-      <c r="N7" t="n">
-        <v>39749</v>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>39750 (esterno)</t>
+        </is>
       </c>
       <c r="O7" t="inlineStr">
         <is>
@@ -976,60 +965,57 @@
         </is>
       </c>
       <c r="P7" t="n">
-        <v>39749</v>
+        <v>39750</v>
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>2025-04-22 00:00:00</t>
+          <t>2025-04-23 00:00:00</t>
         </is>
       </c>
       <c r="R7" s="1" t="n">
-        <v>-1.471584467118056</v>
-      </c>
-      <c r="S7" s="1" t="n">
-        <v>-0.4161458333333333</v>
-      </c>
-      <c r="T7" t="n">
-        <v>4</v>
+        <v>-19.37171361502315</v>
+      </c>
+      <c r="S7" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>250923</v>
+        <v>251456</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>R10</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="D8" t="n">
-        <v>109.46875</v>
+        <v>147.5245901639344</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2025-05-07 09:59:15</t>
+          <t>2025-05-08 07:00:00</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>2025-05-07 10:31:15</t>
+          <t>2025-05-08 07:25:00</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>2025-05-07 10:31:15</t>
+          <t>2025-05-08 07:25:00</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>2025-05-07 12:20:43</t>
+          <t>2025-05-08 09:52:31</t>
         </is>
       </c>
       <c r="I8" t="n">
-        <v>7006</v>
+        <v>8999</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
@@ -1038,17 +1024,17 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L8" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="M8" t="n">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="N8" t="n">
-        <v>39749</v>
+        <v>39746</v>
       </c>
       <c r="O8" t="inlineStr">
         <is>
@@ -1056,60 +1042,57 @@
         </is>
       </c>
       <c r="P8" t="n">
-        <v>39749</v>
+        <v>39746</v>
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>2025-04-07 00:00:00</t>
+          <t>2025-05-09 00:00:00</t>
         </is>
       </c>
       <c r="R8" s="1" t="n">
-        <v>-1.446853298611111</v>
-      </c>
-      <c r="S8" s="1" t="n">
-        <v>-0.5143880208333333</v>
-      </c>
-      <c r="T8" t="n">
-        <v>2</v>
+        <v>-2.411475409837963</v>
+      </c>
+      <c r="S8" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>251455</v>
+        <v>251371</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>R10</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="D9" t="n">
-        <v>82.765625</v>
+        <v>0</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>2025-05-07 12:20:43</t>
+          <t>2025-05-08 09:52:31</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>2025-05-07 12:52:43</t>
+          <t>2025-05-08 10:17:31</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>2025-05-07 12:52:43</t>
+          <t>2025-05-08 10:17:31</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>2025-05-07 14:15:29</t>
+          <t>2025-05-08 10:17:31</t>
         </is>
       </c>
       <c r="I9" t="n">
-        <v>5297</v>
+        <v>0</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
@@ -1127,8 +1110,10 @@
       <c r="M9" t="n">
         <v>70</v>
       </c>
-      <c r="N9" t="n">
-        <v>39749</v>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>39666 (esterno)</t>
+        </is>
       </c>
       <c r="O9" t="inlineStr">
         <is>
@@ -1136,60 +1121,57 @@
         </is>
       </c>
       <c r="P9" t="n">
-        <v>39749</v>
+        <v>39666</v>
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>2025-04-15 00:00:00</t>
+          <t>2025-04-24 00:00:00</t>
         </is>
       </c>
       <c r="R9" s="1" t="n">
-        <v>-0.3623372395833334</v>
-      </c>
-      <c r="S9" s="1" t="n">
-        <v>-0.5940863715277778</v>
-      </c>
-      <c r="T9" t="n">
+        <v>-14.42883652094907</v>
+      </c>
+      <c r="S9" t="n">
         <v>7</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>251371</v>
+        <v>251742</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>R10</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D10" t="n">
-        <v>0</v>
+        <v>134.8524590163935</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2025-05-07 14:15:29</t>
+          <t>2025-05-08 10:17:31</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>2025-05-07 14:30:29</t>
+          <t>2025-05-08 10:37:31</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>2025-05-07 14:30:29</t>
+          <t>2025-05-08 10:37:31</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>2025-05-07 14:30:29</t>
+          <t>2025-05-08 12:52:22</t>
         </is>
       </c>
       <c r="I10" t="n">
-        <v>0</v>
+        <v>8226</v>
       </c>
       <c r="J10" t="inlineStr">
         <is>
@@ -1207,10 +1189,8 @@
       <c r="M10" t="n">
         <v>70</v>
       </c>
-      <c r="N10" t="inlineStr">
-        <is>
-          <t>39666 (esterno)</t>
-        </is>
+      <c r="N10" t="n">
+        <v>39749</v>
       </c>
       <c r="O10" t="inlineStr">
         <is>
@@ -1218,60 +1198,57 @@
         </is>
       </c>
       <c r="P10" t="n">
-        <v>39666</v>
+        <v>39749</v>
       </c>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>2025-04-24 00:00:00</t>
+          <t>2025-05-15 00:00:00</t>
         </is>
       </c>
       <c r="R10" s="1" t="n">
-        <v>-13.48732638888889</v>
-      </c>
-      <c r="S10" s="1" t="n">
-        <v>-13.60450303819444</v>
-      </c>
-      <c r="T10" t="n">
+        <v>-1.536372950821759</v>
+      </c>
+      <c r="S10" t="n">
         <v>7</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>251395</v>
+        <v>251840</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>R10</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="D11" t="n">
-        <v>35.34375</v>
+        <v>93.67213114754098</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>2025-05-07 14:30:29</t>
+          <t>2025-05-08 12:52:22</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>2025-05-07 14:49:29</t>
+          <t>2025-05-08 13:17:22</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>2025-05-07 14:49:29</t>
+          <t>2025-05-08 13:17:22</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>2025-05-08 07:24:49</t>
+          <t>2025-05-08 14:51:02</t>
         </is>
       </c>
       <c r="I11" t="n">
-        <v>2262</v>
+        <v>5714</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
@@ -1284,13 +1261,13 @@
         </is>
       </c>
       <c r="L11" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="M11" t="n">
         <v>70</v>
       </c>
       <c r="N11" t="n">
-        <v>39749</v>
+        <v>39758</v>
       </c>
       <c r="O11" t="inlineStr">
         <is>
@@ -1298,60 +1275,57 @@
         </is>
       </c>
       <c r="P11" t="n">
-        <v>39749</v>
+        <v>39758</v>
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>2025-04-23 00:00:00</t>
+          <t>2025-05-09 00:00:00</t>
         </is>
       </c>
       <c r="R11" s="1" t="n">
-        <v>-0.4741319444444445</v>
-      </c>
-      <c r="S11" s="1" t="n">
-        <v>-1.308908420138889</v>
-      </c>
-      <c r="T11" t="n">
-        <v>7</v>
+        <v>-0.6187841530092593</v>
+      </c>
+      <c r="S11" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>251396</v>
+        <v>251229</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>R10</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="D12" t="n">
-        <v>35.34375</v>
+        <v>307.1967213114754</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>2025-05-08 07:24:49</t>
+          <t>2025-05-08 14:51:02</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>2025-05-08 07:39:49</t>
+          <t>2025-05-09 07:16:02</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>2025-05-08 07:39:49</t>
+          <t>2025-05-09 07:16:02</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>2025-05-08 08:15:10</t>
+          <t>2025-05-09 12:23:14</t>
         </is>
       </c>
       <c r="I12" t="n">
-        <v>2262</v>
+        <v>18739</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
@@ -1360,7 +1334,7 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R9</t>
         </is>
       </c>
       <c r="L12" t="n">
@@ -1369,8 +1343,10 @@
       <c r="M12" t="n">
         <v>70</v>
       </c>
-      <c r="N12" t="n">
-        <v>39749</v>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>39723 (esterno)</t>
+        </is>
       </c>
       <c r="O12" t="inlineStr">
         <is>
@@ -1378,60 +1354,57 @@
         </is>
       </c>
       <c r="P12" t="n">
-        <v>39749</v>
+        <v>39723</v>
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>2025-05-02 00:00:00</t>
+          <t>2025-05-15 00:00:00</t>
         </is>
       </c>
       <c r="R12" s="1" t="n">
-        <v>-0.5250651041666666</v>
-      </c>
-      <c r="S12" s="1" t="n">
-        <v>-1.343869357638889</v>
-      </c>
-      <c r="T12" t="n">
-        <v>7</v>
+        <v>0</v>
+      </c>
+      <c r="S12" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>251548</v>
+        <v>251225</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>R12</t>
         </is>
       </c>
       <c r="C13" t="n">
         <v>19</v>
       </c>
       <c r="D13" t="n">
-        <v>206.90625</v>
+        <v>0</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>2025-05-08 08:15:10</t>
+          <t>2025-05-08 12:00:00</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>2025-05-08 08:34:10</t>
+          <t>2025-05-08 12:19:00</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>2025-05-08 08:34:10</t>
+          <t>2025-05-08 12:19:00</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>2025-05-08 12:01:04</t>
+          <t>2025-05-08 12:19:00</t>
         </is>
       </c>
       <c r="I13" t="n">
-        <v>13242</v>
+        <v>0</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
@@ -1440,17 +1413,17 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
         </is>
       </c>
       <c r="L13" t="n">
         <v>4</v>
       </c>
       <c r="M13" t="n">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="N13" t="n">
-        <v>39749</v>
+        <v>39747</v>
       </c>
       <c r="O13" t="inlineStr">
         <is>
@@ -1458,60 +1431,57 @@
         </is>
       </c>
       <c r="P13" t="n">
-        <v>39749</v>
+        <v>39747</v>
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>2025-05-06 00:00:00</t>
+          <t>2025-04-30 00:00:00</t>
         </is>
       </c>
       <c r="R13" s="1" t="n">
-        <v>-1.348611111111111</v>
-      </c>
-      <c r="S13" s="1" t="n">
-        <v>-1.500748697916667</v>
-      </c>
-      <c r="T13" t="n">
-        <v>7</v>
+        <v>-0.5131944444444444</v>
+      </c>
+      <c r="S13" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>251477</v>
+        <v>251227</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>R12</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="D14" t="n">
-        <v>468.734375</v>
+        <v>0</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>2025-05-08 12:01:04</t>
+          <t>2025-05-08 12:19:00</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>2025-05-08 12:33:04</t>
+          <t>2025-05-08 12:34:00</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>2025-05-08 12:33:04</t>
+          <t>2025-05-08 12:34:00</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>2025-05-09 12:21:48</t>
+          <t>2025-05-08 12:34:00</t>
         </is>
       </c>
       <c r="I14" t="n">
-        <v>29999</v>
+        <v>0</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
@@ -1520,17 +1490,17 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
         </is>
       </c>
       <c r="L14" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M14" t="n">
         <v>76</v>
       </c>
       <c r="N14" t="n">
-        <v>39760</v>
+        <v>39746</v>
       </c>
       <c r="O14" t="inlineStr">
         <is>
@@ -1538,60 +1508,57 @@
         </is>
       </c>
       <c r="P14" t="n">
-        <v>39760</v>
+        <v>39746</v>
       </c>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>2025-04-28 00:00:00</t>
+          <t>2025-05-05 00:00:00</t>
         </is>
       </c>
       <c r="R14" s="1" t="n">
-        <v>-2.452224392361111</v>
-      </c>
-      <c r="S14" s="1" t="n">
-        <v>-2.515147569444444</v>
-      </c>
-      <c r="T14" t="n">
+        <v>-2.523611111111111</v>
+      </c>
+      <c r="S14" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>251050</v>
+        <v>251547</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>217</v>
+        <v>19</v>
       </c>
       <c r="D15" t="n">
-        <v>0</v>
+        <v>205.140625</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>2025-05-09 07:00:00</t>
+          <t>2025-05-07 07:00:00</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>2025-05-09 10:37:00</t>
+          <t>2025-05-07 07:19:00</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>2025-05-09 10:37:00</t>
+          <t>2025-05-07 07:19:00</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>2025-05-09 10:37:00</t>
+          <t>2025-05-07 10:44:08</t>
         </is>
       </c>
       <c r="I15" t="n">
-        <v>0</v>
+        <v>13129</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
@@ -1600,17 +1567,17 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L15" t="n">
-        <v>38</v>
+        <v>4</v>
       </c>
       <c r="M15" t="n">
         <v>70</v>
       </c>
       <c r="N15" t="n">
-        <v>39747</v>
+        <v>39749</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
@@ -1618,60 +1585,57 @@
         </is>
       </c>
       <c r="P15" t="n">
-        <v>39747</v>
+        <v>39749</v>
       </c>
       <c r="Q15" t="inlineStr">
         <is>
-          <t>2025-04-16 00:00:00</t>
+          <t>2025-05-06 00:00:00</t>
         </is>
       </c>
       <c r="R15" s="1" t="n">
-        <v>-1.442361111111111</v>
-      </c>
-      <c r="S15" s="1" t="n">
-        <v>-1.442361111111111</v>
-      </c>
-      <c r="T15" t="n">
-        <v>2</v>
+        <v>-0.4473198784722222</v>
+      </c>
+      <c r="S15" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>251054</v>
+        <v>251455</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="D16" t="n">
-        <v>0</v>
+        <v>82.765625</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>2025-05-09 10:37:00</t>
+          <t>2025-05-07 10:44:08</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>2025-05-09 11:12:00</t>
+          <t>2025-05-07 10:59:08</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>2025-05-09 11:12:00</t>
+          <t>2025-05-07 10:59:08</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>2025-05-09 11:12:00</t>
+          <t>2025-05-07 12:21:54</t>
         </is>
       </c>
       <c r="I16" t="n">
-        <v>0</v>
+        <v>5297</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
@@ -1680,17 +1644,17 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L16" t="n">
-        <v>38</v>
+        <v>4</v>
       </c>
       <c r="M16" t="n">
         <v>70</v>
       </c>
       <c r="N16" t="n">
-        <v>39747</v>
+        <v>39749</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
@@ -1698,60 +1662,57 @@
         </is>
       </c>
       <c r="P16" t="n">
-        <v>39747</v>
+        <v>39749</v>
       </c>
       <c r="Q16" t="inlineStr">
         <is>
-          <t>2025-04-16 00:00:00</t>
+          <t>2025-04-15 00:00:00</t>
         </is>
       </c>
       <c r="R16" s="1" t="n">
-        <v>-1.466666666666667</v>
-      </c>
-      <c r="S16" s="1" t="n">
-        <v>-1.466666666666667</v>
-      </c>
-      <c r="T16" t="n">
-        <v>2</v>
+        <v>-0.5152126736111111</v>
+      </c>
+      <c r="S16" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>251081</v>
+        <v>251391</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>125</v>
+        <v>17</v>
       </c>
       <c r="D17" t="n">
-        <v>42.42253521126761</v>
+        <v>91.640625</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>2025-05-09 11:12:00</t>
+          <t>2025-05-07 12:21:54</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>2025-05-09 13:17:00</t>
+          <t>2025-05-07 12:38:54</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>2025-05-09 13:17:00</t>
+          <t>2025-05-07 12:38:54</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>2025-05-09 13:59:25</t>
+          <t>2025-05-07 14:10:32</t>
         </is>
       </c>
       <c r="I17" t="n">
-        <v>3012</v>
+        <v>5865</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
@@ -1760,19 +1721,17 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L17" t="n">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="M17" t="n">
         <v>70</v>
       </c>
-      <c r="N17" t="inlineStr">
-        <is>
-          <t>39750 (esterno)</t>
-        </is>
+      <c r="N17" t="n">
+        <v>39749</v>
       </c>
       <c r="O17" t="inlineStr">
         <is>
@@ -1780,7 +1739,7 @@
         </is>
       </c>
       <c r="P17" t="n">
-        <v>39750</v>
+        <v>39749</v>
       </c>
       <c r="Q17" t="inlineStr">
         <is>
@@ -1788,52 +1747,49 @@
         </is>
       </c>
       <c r="R17" s="1" t="n">
-        <v>-16.58293231612268</v>
-      </c>
-      <c r="S17" s="1" t="n">
-        <v>-16.58293231612268</v>
-      </c>
-      <c r="T17" t="n">
-        <v>2</v>
+        <v>-0.5906575520833334</v>
+      </c>
+      <c r="S17" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>251284</v>
+        <v>251395</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>CASON</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>40.5</v>
+        <v>17</v>
       </c>
       <c r="D18" t="n">
-        <v>297.0909090909091</v>
+        <v>35.34375</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>2025-05-09 07:00:00</t>
+          <t>2025-05-07 14:10:32</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>2025-05-09 07:40:30</t>
+          <t>2025-05-07 14:27:32</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>2025-05-09 07:40:30</t>
+          <t>2025-05-07 14:27:32</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>2025-05-09 12:37:35</t>
+          <t>2025-05-08 07:02:53</t>
         </is>
       </c>
       <c r="I18" t="n">
-        <v>16340</v>
+        <v>2262</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
@@ -1842,17 +1798,17 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>CASON ;R6</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L18" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="M18" t="n">
         <v>70</v>
       </c>
       <c r="N18" t="n">
-        <v>39747</v>
+        <v>39749</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
@@ -1860,81 +1816,76 @@
         </is>
       </c>
       <c r="P18" t="n">
-        <v>39747</v>
+        <v>39749</v>
       </c>
       <c r="Q18" t="inlineStr">
         <is>
-          <t>2025-05-12 00:00:00</t>
+          <t>2025-04-23 00:00:00</t>
         </is>
       </c>
       <c r="R18" s="1" t="n">
-        <v>-1.526104797974537</v>
-      </c>
-      <c r="S18" s="1" t="n">
-        <v>-1.526104797974537</v>
-      </c>
-      <c r="T18" t="n">
-        <v>1</v>
+        <v>-1.293674045138889</v>
+      </c>
+      <c r="S18" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>251706</v>
+        <v>251396</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>T3</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="D19" t="n">
-        <v>50.79365079365079</v>
+        <v>35.34375</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>2025-05-12 07:00:00</t>
+          <t>2025-05-08 07:02:53</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>2025-05-12 07:00:00</t>
+          <t>2025-05-08 07:17:53</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>2025-05-12 07:00:00</t>
+          <t>2025-05-08 07:17:53</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>2025-05-12 07:50:47</t>
+          <t>2025-05-08 07:53:14</t>
         </is>
       </c>
       <c r="I19" t="n">
-        <v>3200</v>
+        <v>2262</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>foglio</t>
+          <t>bobina</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>T3</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L19" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="M19" t="n">
-        <v>0</v>
-      </c>
-      <c r="N19" t="inlineStr">
-        <is>
-          <t>39764 (esterno)</t>
-        </is>
+        <v>70</v>
+      </c>
+      <c r="N19" t="n">
+        <v>39749</v>
       </c>
       <c r="O19" t="inlineStr">
         <is>
@@ -1942,60 +1893,57 @@
         </is>
       </c>
       <c r="P19" t="n">
-        <v>39764</v>
+        <v>39749</v>
       </c>
       <c r="Q19" t="inlineStr">
         <is>
-          <t>2025-05-14 00:00:00</t>
+          <t>2025-05-02 00:00:00</t>
         </is>
       </c>
       <c r="R19" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="S19" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="T19" t="n">
+        <v>-1.328634982638889</v>
+      </c>
+      <c r="S19" t="n">
         <v>7</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>251547</v>
+        <v>251548</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>BIMEC 5</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="D20" t="n">
-        <v>184.9154929577465</v>
+        <v>206.90625</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>2025-05-08 07:00:00</t>
+          <t>2025-05-08 07:53:14</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>2025-05-08 07:34:00</t>
+          <t>2025-05-08 08:12:14</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>2025-05-08 07:34:00</t>
+          <t>2025-05-08 08:12:14</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>2025-05-08 10:38:54</t>
+          <t>2025-05-08 11:39:08</t>
         </is>
       </c>
       <c r="I20" t="n">
-        <v>13129</v>
+        <v>13242</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
@@ -2030,52 +1978,49 @@
         </is>
       </c>
       <c r="R20" s="1" t="n">
-        <v>-1.443691314548611</v>
-      </c>
-      <c r="S20" s="1" t="n">
-        <v>-1.443691314548611</v>
-      </c>
-      <c r="T20" t="n">
+        <v>-1.485514322916667</v>
+      </c>
+      <c r="S20" t="n">
         <v>7</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>251225</v>
+        <v>250894</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>BIMEC 5</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D21" t="n">
-        <v>0</v>
+        <v>691.59375</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>2025-05-08 10:38:54</t>
+          <t>2025-05-08 11:39:08</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>2025-05-08 11:08:54</t>
+          <t>2025-05-08 12:11:08</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>2025-05-08 11:08:54</t>
+          <t>2025-05-08 12:11:08</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>2025-05-08 11:08:54</t>
+          <t>2025-05-12 07:42:44</t>
         </is>
       </c>
       <c r="I21" t="n">
-        <v>0</v>
+        <v>44262</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
@@ -2084,78 +2029,73 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L21" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M21" t="n">
         <v>76</v>
       </c>
       <c r="N21" t="n">
-        <v>39747</v>
-      </c>
-      <c r="O21" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
+        <v>39755</v>
+      </c>
+      <c r="O21" t="n">
+        <v>0</v>
       </c>
       <c r="P21" t="n">
-        <v>39747</v>
+        <v>0</v>
       </c>
       <c r="Q21" t="inlineStr">
         <is>
-          <t>2025-04-30 00:00:00</t>
+          <t>2025-05-05 00:00:00</t>
         </is>
       </c>
       <c r="R21" s="1" t="n">
-        <v>-0.5131944444444444</v>
-      </c>
-      <c r="S21" s="1" t="n">
-        <v>-0.4645246478819445</v>
-      </c>
-      <c r="T21" t="n">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="S21" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>250759</v>
+        <v>250923</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>BIMEC 5</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C22" t="n">
         <v>15</v>
       </c>
       <c r="D22" t="n">
-        <v>118.2816901408451</v>
+        <v>109.46875</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>2025-05-08 11:08:54</t>
+          <t>2025-05-12 07:42:44</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>2025-05-08 11:23:54</t>
+          <t>2025-05-12 07:57:44</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>2025-05-08 11:23:54</t>
+          <t>2025-05-12 07:57:44</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>2025-05-08 13:22:11</t>
+          <t>2025-05-12 09:47:12</t>
         </is>
       </c>
       <c r="I22" t="n">
-        <v>8398</v>
+        <v>7006</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
@@ -2164,17 +2104,17 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
         </is>
       </c>
       <c r="L22" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M22" t="n">
         <v>76</v>
       </c>
       <c r="N22" t="n">
-        <v>39747</v>
+        <v>39749</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
@@ -2182,60 +2122,57 @@
         </is>
       </c>
       <c r="P22" t="n">
-        <v>39747</v>
+        <v>39749</v>
       </c>
       <c r="Q22" t="inlineStr">
         <is>
-          <t>2025-03-13 00:00:00</t>
+          <t>2025-04-07 00:00:00</t>
         </is>
       </c>
       <c r="R22" s="1" t="n">
-        <v>-0.5466647104861111</v>
-      </c>
-      <c r="S22" s="1" t="n">
-        <v>-0.5570813771527778</v>
-      </c>
-      <c r="T22" t="n">
-        <v>1</v>
+        <v>-5.407779947916667</v>
+      </c>
+      <c r="S22" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>250894</v>
+        <v>251477</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>BIMEC 5</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D23" t="n">
-        <v>623.4084507042254</v>
+        <v>468.734375</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>2025-05-08 13:22:11</t>
+          <t>2025-05-12 09:47:12</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>2025-05-08 13:39:11</t>
+          <t>2025-05-12 10:06:12</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>2025-05-08 13:39:11</t>
+          <t>2025-05-12 10:06:12</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>2025-05-12 08:02:36</t>
+          <t>2025-05-13 09:54:56</t>
         </is>
       </c>
       <c r="I23" t="n">
-        <v>44262</v>
+        <v>29999</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
@@ -2244,76 +2181,75 @@
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L23" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="M23" t="n">
         <v>76</v>
       </c>
       <c r="N23" t="n">
-        <v>39755</v>
-      </c>
-      <c r="O23" t="n">
-        <v>0</v>
+        <v>39760</v>
+      </c>
+      <c r="O23" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
       </c>
       <c r="P23" t="n">
-        <v>0</v>
+        <v>39760</v>
       </c>
       <c r="Q23" t="inlineStr">
         <is>
-          <t>2025-05-05 00:00:00</t>
+          <t>2025-04-28 00:00:00</t>
         </is>
       </c>
       <c r="R23" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="S23" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="T23" t="n">
-        <v>4</v>
+        <v>-6.413151041666667</v>
+      </c>
+      <c r="S23" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>251456</v>
+        <v>251782</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>R3</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="D24" t="n">
-        <v>183.6530612244898</v>
+        <v>188.640625</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>2025-05-08 07:00:00</t>
+          <t>2025-05-13 09:54:56</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>2025-05-08 07:40:00</t>
+          <t>2025-05-13 10:09:56</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>2025-05-08 07:40:00</t>
+          <t>2025-05-13 10:09:56</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>2025-05-08 10:43:39</t>
+          <t>2025-05-13 13:18:34</t>
         </is>
       </c>
       <c r="I24" t="n">
-        <v>8999</v>
+        <v>12073</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
@@ -2322,17 +2258,17 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L24" t="n">
         <v>3</v>
       </c>
       <c r="M24" t="n">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="N24" t="n">
-        <v>39746</v>
+        <v>39754</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
@@ -2340,60 +2276,57 @@
         </is>
       </c>
       <c r="P24" t="n">
-        <v>39746</v>
+        <v>39754</v>
       </c>
       <c r="Q24" t="inlineStr">
         <is>
-          <t>2025-05-09 00:00:00</t>
+          <t>2025-05-16 00:00:00</t>
         </is>
       </c>
       <c r="R24" s="1" t="n">
-        <v>-3.300510204085648</v>
-      </c>
-      <c r="S24" s="1" t="n">
-        <v>-2.446981292511574</v>
-      </c>
-      <c r="T24" t="n">
+        <v>-4.554568142361111</v>
+      </c>
+      <c r="S24" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>251416</v>
+        <v>251284</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>R3</t>
+          <t>CASON</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>40</v>
+        <v>40.5</v>
       </c>
       <c r="D25" t="n">
-        <v>229.0204081632653</v>
+        <v>297.0909090909091</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>2025-05-08 10:43:39</t>
+          <t>2025-05-09 07:00:00</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>2025-05-08 11:23:39</t>
+          <t>2025-05-09 07:40:30</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>2025-05-08 11:23:39</t>
+          <t>2025-05-09 07:40:30</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>2025-05-09 07:12:40</t>
+          <t>2025-05-09 12:37:35</t>
         </is>
       </c>
       <c r="I25" t="n">
-        <v>11222</v>
+        <v>16340</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
@@ -2402,76 +2335,75 @@
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>CASON ;R6</t>
         </is>
       </c>
       <c r="L25" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="M25" t="n">
         <v>70</v>
       </c>
       <c r="N25" t="n">
-        <v>39755</v>
-      </c>
-      <c r="O25" t="n">
-        <v>0</v>
+        <v>39747</v>
+      </c>
+      <c r="O25" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
       </c>
       <c r="P25" t="n">
-        <v>0</v>
+        <v>39747</v>
       </c>
       <c r="Q25" t="inlineStr">
         <is>
-          <t>2025-04-23 00:00:00</t>
+          <t>2025-05-12 00:00:00</t>
         </is>
       </c>
       <c r="R25" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="S25" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="T25" t="n">
-        <v>2</v>
+        <v>-1.526104797974537</v>
+      </c>
+      <c r="S25" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>251227</v>
+        <v>251651</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>R12</t>
+          <t>BIMEC 4</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="D26" t="n">
-        <v>0</v>
+        <v>767.7049180327868</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>2025-05-08 12:00:00</t>
+          <t>2025-05-09 07:00:00</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>2025-05-08 12:19:00</t>
+          <t>2025-05-09 07:29:00</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>2025-05-08 12:19:00</t>
+          <t>2025-05-09 07:29:00</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>2025-05-08 12:19:00</t>
+          <t>2025-05-12 12:16:42</t>
         </is>
       </c>
       <c r="I26" t="n">
-        <v>0</v>
+        <v>46830</v>
       </c>
       <c r="J26" t="inlineStr">
         <is>
@@ -2480,78 +2412,73 @@
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L26" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M26" t="n">
         <v>76</v>
       </c>
       <c r="N26" t="n">
-        <v>39746</v>
-      </c>
-      <c r="O26" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
+        <v>39755</v>
+      </c>
+      <c r="O26" t="n">
+        <v>0</v>
       </c>
       <c r="P26" t="n">
-        <v>39746</v>
+        <v>0</v>
       </c>
       <c r="Q26" t="inlineStr">
         <is>
-          <t>2025-05-05 00:00:00</t>
+          <t>2025-05-12 00:00:00</t>
         </is>
       </c>
       <c r="R26" s="1" t="n">
-        <v>-2.523611111111111</v>
-      </c>
-      <c r="S26" s="1" t="n">
-        <v>-2.513194444444444</v>
-      </c>
-      <c r="T26" t="n">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="S26" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>251782</v>
+        <v>251416</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>R12</t>
+          <t>R3</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="D27" t="n">
-        <v>170.0422535211268</v>
+        <v>229.0204081632653</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>2025-05-08 12:19:00</t>
+          <t>2025-05-08 07:00:00</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>2025-05-08 12:36:00</t>
+          <t>2025-05-08 07:35:00</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>2025-05-08 12:36:00</t>
+          <t>2025-05-08 07:35:00</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>2025-05-09 07:26:02</t>
+          <t>2025-05-08 11:24:01</t>
         </is>
       </c>
       <c r="I27" t="n">
-        <v>12073</v>
+        <v>11222</v>
       </c>
       <c r="J27" t="inlineStr">
         <is>
@@ -2560,39 +2487,34 @@
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L27" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M27" t="n">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="N27" t="n">
-        <v>39754</v>
-      </c>
-      <c r="O27" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
+        <v>39755</v>
+      </c>
+      <c r="O27" t="n">
+        <v>0</v>
       </c>
       <c r="P27" t="n">
-        <v>39754</v>
+        <v>0</v>
       </c>
       <c r="Q27" t="inlineStr">
         <is>
-          <t>2025-05-16 00:00:00</t>
+          <t>2025-04-23 00:00:00</t>
         </is>
       </c>
       <c r="R27" s="1" t="n">
-        <v>-0.3201682316087963</v>
-      </c>
-      <c r="S27" s="1" t="n">
-        <v>-0.3097515649421296</v>
-      </c>
-      <c r="T27" t="n">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="S27" t="n">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Non va ancora nulla oltre LS1
</commit_message>
<xml_diff>
--- a/PS-VRP/Dati_output/insert_inter.xlsx
+++ b/PS-VRP/Dati_output/insert_inter.xlsx
@@ -515,60 +515,62 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>251227</v>
+        <v>251706</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>BIMEC 5</t>
+          <t>T3</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
+        <v>50.79365079365079</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>2025-05-12 07:00:00</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>2025-05-12 07:00:00</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>2025-05-12 07:00:00</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>2025-05-12 07:50:47</t>
+        </is>
+      </c>
+      <c r="I2" t="n">
+        <v>3200</v>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>foglio</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>T3</t>
+        </is>
+      </c>
+      <c r="L2" t="n">
         <v>0</v>
       </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>2025-05-08 07:00:00</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>2025-05-08 07:19:00</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>2025-05-08 07:19:00</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>2025-05-08 07:19:00</t>
-        </is>
-      </c>
-      <c r="I2" t="n">
+      <c r="M2" t="n">
         <v>0</v>
       </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>bobina</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
-        </is>
-      </c>
-      <c r="L2" t="n">
-        <v>4</v>
-      </c>
-      <c r="M2" t="n">
-        <v>76</v>
-      </c>
-      <c r="N2" t="n">
-        <v>39746</v>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>39764 (esterno)</t>
+        </is>
       </c>
       <c r="O2" t="inlineStr">
         <is>
@@ -576,53 +578,53 @@
         </is>
       </c>
       <c r="P2" t="n">
-        <v>39746</v>
+        <v>39764</v>
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>2025-05-05 00:00:00</t>
+          <t>2025-05-14 00:00:00</t>
         </is>
       </c>
       <c r="R2" s="1" t="n">
-        <v>-2.304861111111111</v>
+        <v>0</v>
       </c>
       <c r="S2" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>251225</v>
+        <v>251050</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>BIMEC 5</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>15</v>
+        <v>217</v>
       </c>
       <c r="D3" t="n">
         <v>0</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2025-05-08 07:19:00</t>
+          <t>2025-05-09 07:00:00</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2025-05-08 07:34:00</t>
+          <t>2025-05-09 10:37:00</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>2025-05-08 07:34:00</t>
+          <t>2025-05-09 10:37:00</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>2025-05-08 07:34:00</t>
+          <t>2025-05-09 10:37:00</t>
         </is>
       </c>
       <c r="I3" t="n">
@@ -635,14 +637,14 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="L3" t="n">
-        <v>4</v>
+        <v>38</v>
       </c>
       <c r="M3" t="n">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="N3" t="n">
         <v>39747</v>
@@ -657,53 +659,53 @@
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>2025-04-30 00:00:00</t>
+          <t>2025-04-16 00:00:00</t>
         </is>
       </c>
       <c r="R3" s="1" t="n">
-        <v>-0.3152777777777778</v>
+        <v>-1.442361111111111</v>
       </c>
       <c r="S3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>251164</v>
+        <v>251054</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>BIMEC 5</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D4" t="n">
-        <v>140.8450704225352</v>
+        <v>0</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2025-05-08 07:34:00</t>
+          <t>2025-05-09 10:37:00</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>2025-05-08 08:08:00</t>
+          <t>2025-05-09 11:12:00</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>2025-05-08 08:08:00</t>
+          <t>2025-05-09 11:12:00</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>2025-05-08 10:28:50</t>
+          <t>2025-05-09 11:12:00</t>
         </is>
       </c>
       <c r="I4" t="n">
-        <v>10000</v>
+        <v>0</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
@@ -712,17 +714,17 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="L4" t="n">
-        <v>6</v>
+        <v>38</v>
       </c>
       <c r="M4" t="n">
         <v>70</v>
       </c>
       <c r="N4" t="n">
-        <v>39749</v>
+        <v>39747</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
@@ -730,57 +732,57 @@
         </is>
       </c>
       <c r="P4" t="n">
-        <v>39749</v>
+        <v>39747</v>
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>2025-04-22 00:00:00</t>
+          <t>2025-04-16 00:00:00</t>
         </is>
       </c>
       <c r="R4" s="1" t="n">
-        <v>-1.436697965567129</v>
+        <v>-1.466666666666667</v>
       </c>
       <c r="S4" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>251547</v>
+        <v>251081</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>BIMEC 5</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>19</v>
+        <v>125</v>
       </c>
       <c r="D5" t="n">
-        <v>184.9154929577465</v>
+        <v>42.42253521126761</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2025-05-08 10:28:50</t>
+          <t>2025-05-09 11:12:00</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>2025-05-08 10:47:50</t>
+          <t>2025-05-09 13:17:00</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>2025-05-08 10:47:50</t>
+          <t>2025-05-09 13:17:00</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>2025-05-08 13:52:45</t>
+          <t>2025-05-09 13:59:25</t>
         </is>
       </c>
       <c r="I5" t="n">
-        <v>13129</v>
+        <v>3012</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
@@ -789,17 +791,19 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="L5" t="n">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="M5" t="n">
         <v>70</v>
       </c>
-      <c r="N5" t="n">
-        <v>39749</v>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>39750 (esterno)</t>
+        </is>
       </c>
       <c r="O5" t="inlineStr">
         <is>
@@ -807,57 +811,57 @@
         </is>
       </c>
       <c r="P5" t="n">
-        <v>39749</v>
+        <v>39750</v>
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>2025-05-06 00:00:00</t>
+          <t>2025-04-23 00:00:00</t>
         </is>
       </c>
       <c r="R5" s="1" t="n">
-        <v>-1.578305946793982</v>
+        <v>-16.58293231612268</v>
       </c>
       <c r="S5" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>250759</v>
+        <v>251284</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>BIMEC 5</t>
+          <t>CASON</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>30</v>
+        <v>40.5</v>
       </c>
       <c r="D6" t="n">
-        <v>118.2816901408451</v>
+        <v>297.0909090909091</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2025-05-08 13:52:45</t>
+          <t>2025-05-09 07:00:00</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2025-05-08 14:22:45</t>
+          <t>2025-05-09 07:40:30</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>2025-05-08 14:22:45</t>
+          <t>2025-05-09 07:40:30</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>2025-05-09 08:21:02</t>
+          <t>2025-05-09 12:37:35</t>
         </is>
       </c>
       <c r="I6" t="n">
-        <v>8398</v>
+        <v>16340</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
@@ -866,14 +870,14 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12</t>
+          <t>CASON ;R6</t>
         </is>
       </c>
       <c r="L6" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="M6" t="n">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="N6" t="n">
         <v>39747</v>
@@ -888,11 +892,11 @@
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>2025-03-13 00:00:00</t>
+          <t>2025-05-12 00:00:00</t>
         </is>
       </c>
       <c r="R6" s="1" t="n">
-        <v>-1.347946009386574</v>
+        <v>-1.526104797974537</v>
       </c>
       <c r="S6" t="n">
         <v>1</v>
@@ -900,41 +904,41 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>250894</v>
+        <v>251742</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>BIMEC 5</t>
+          <t>R10</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="D7" t="n">
-        <v>623.4084507042254</v>
+        <v>134.8524590163935</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2025-05-09 08:21:02</t>
+          <t>2025-05-08 07:00:00</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>2025-05-09 08:38:02</t>
+          <t>2025-05-08 07:30:00</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>2025-05-09 08:38:02</t>
+          <t>2025-05-08 07:30:00</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>2025-05-12 11:01:27</t>
+          <t>2025-05-08 09:44:51</t>
         </is>
       </c>
       <c r="I7" t="n">
-        <v>44262</v>
+        <v>8226</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
@@ -943,94 +947,94 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L7" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M7" t="n">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="N7" t="n">
-        <v>39755</v>
-      </c>
-      <c r="O7" t="n">
-        <v>0</v>
+        <v>39749</v>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
       </c>
       <c r="P7" t="n">
-        <v>0</v>
+        <v>39749</v>
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>2025-05-05 00:00:00</t>
+          <t>2025-05-15 00:00:00</t>
         </is>
       </c>
       <c r="R7" s="1" t="n">
-        <v>0</v>
+        <v>-1.406147540983796</v>
       </c>
       <c r="S7" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>251706</v>
+        <v>251164</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>T3</t>
+          <t>R10</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="D8" t="n">
-        <v>50.79365079365079</v>
+        <v>163.9344262295082</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2025-05-12 07:00:00</t>
+          <t>2025-05-08 09:44:51</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>2025-05-12 07:00:00</t>
+          <t>2025-05-08 10:14:51</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>2025-05-12 07:00:00</t>
+          <t>2025-05-08 10:14:51</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>2025-05-12 07:50:47</t>
+          <t>2025-05-08 12:58:47</t>
         </is>
       </c>
       <c r="I8" t="n">
-        <v>3200</v>
+        <v>10000</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>foglio</t>
+          <t>bobina</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>T3</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L8" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="M8" t="n">
-        <v>0</v>
-      </c>
-      <c r="N8" t="inlineStr">
-        <is>
-          <t>39764 (esterno)</t>
-        </is>
+        <v>70</v>
+      </c>
+      <c r="N8" t="n">
+        <v>39749</v>
       </c>
       <c r="O8" t="inlineStr">
         <is>
@@ -1038,57 +1042,57 @@
         </is>
       </c>
       <c r="P8" t="n">
-        <v>39764</v>
+        <v>39749</v>
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>2025-05-14 00:00:00</t>
+          <t>2025-04-22 00:00:00</t>
         </is>
       </c>
       <c r="R8" s="1" t="n">
-        <v>0</v>
+        <v>-1.540824225868056</v>
       </c>
       <c r="S8" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>251050</v>
+        <v>251840</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>R10</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>217</v>
+        <v>25</v>
       </c>
       <c r="D9" t="n">
-        <v>0</v>
+        <v>93.67213114754098</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>2025-05-09 07:00:00</t>
+          <t>2025-05-08 12:58:47</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>2025-05-09 10:37:00</t>
+          <t>2025-05-08 13:23:47</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>2025-05-09 10:37:00</t>
+          <t>2025-05-08 13:23:47</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>2025-05-09 10:37:00</t>
+          <t>2025-05-08 14:57:27</t>
         </is>
       </c>
       <c r="I9" t="n">
-        <v>0</v>
+        <v>5714</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
@@ -1097,17 +1101,17 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L9" t="n">
-        <v>38</v>
+        <v>5</v>
       </c>
       <c r="M9" t="n">
         <v>70</v>
       </c>
       <c r="N9" t="n">
-        <v>39747</v>
+        <v>39758</v>
       </c>
       <c r="O9" t="inlineStr">
         <is>
@@ -1115,57 +1119,57 @@
         </is>
       </c>
       <c r="P9" t="n">
-        <v>39747</v>
+        <v>39758</v>
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>2025-04-16 00:00:00</t>
+          <t>2025-05-09 00:00:00</t>
         </is>
       </c>
       <c r="R9" s="1" t="n">
-        <v>-1.442361111111111</v>
+        <v>-0.6232354280555555</v>
       </c>
       <c r="S9" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>251054</v>
+        <v>251229</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>R10</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="D10" t="n">
-        <v>0</v>
+        <v>307.1967213114754</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2025-05-09 10:37:00</t>
+          <t>2025-05-08 14:57:27</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>2025-05-09 11:12:00</t>
+          <t>2025-05-09 07:22:27</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>2025-05-09 11:12:00</t>
+          <t>2025-05-09 07:22:27</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>2025-05-09 11:12:00</t>
+          <t>2025-05-09 12:29:39</t>
         </is>
       </c>
       <c r="I10" t="n">
-        <v>0</v>
+        <v>18739</v>
       </c>
       <c r="J10" t="inlineStr">
         <is>
@@ -1174,17 +1178,19 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R9</t>
         </is>
       </c>
       <c r="L10" t="n">
-        <v>38</v>
+        <v>6</v>
       </c>
       <c r="M10" t="n">
         <v>70</v>
       </c>
-      <c r="N10" t="n">
-        <v>39747</v>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>39723 (esterno)</t>
+        </is>
       </c>
       <c r="O10" t="inlineStr">
         <is>
@@ -1192,57 +1198,57 @@
         </is>
       </c>
       <c r="P10" t="n">
-        <v>39747</v>
+        <v>39723</v>
       </c>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>2025-04-16 00:00:00</t>
+          <t>2025-05-15 00:00:00</t>
         </is>
       </c>
       <c r="R10" s="1" t="n">
-        <v>-1.466666666666667</v>
+        <v>0</v>
       </c>
       <c r="S10" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>251081</v>
+        <v>251782</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>R12</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>125</v>
+        <v>17</v>
       </c>
       <c r="D11" t="n">
-        <v>42.42253521126761</v>
+        <v>170.0422535211268</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>2025-05-09 11:12:00</t>
+          <t>2025-05-08 12:00:00</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>2025-05-09 13:17:00</t>
+          <t>2025-05-08 12:17:00</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>2025-05-09 13:17:00</t>
+          <t>2025-05-08 12:17:00</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>2025-05-09 13:59:25</t>
+          <t>2025-05-09 07:07:02</t>
         </is>
       </c>
       <c r="I11" t="n">
-        <v>3012</v>
+        <v>12073</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
@@ -1251,19 +1257,17 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L11" t="n">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="M11" t="n">
-        <v>70</v>
-      </c>
-      <c r="N11" t="inlineStr">
-        <is>
-          <t>39750 (esterno)</t>
-        </is>
+        <v>76</v>
+      </c>
+      <c r="N11" t="n">
+        <v>39754</v>
       </c>
       <c r="O11" t="inlineStr">
         <is>
@@ -1271,34 +1275,34 @@
         </is>
       </c>
       <c r="P11" t="n">
-        <v>39750</v>
+        <v>39754</v>
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>2025-04-23 00:00:00</t>
+          <t>2025-05-16 00:00:00</t>
         </is>
       </c>
       <c r="R11" s="1" t="n">
-        <v>-16.58293231612268</v>
+        <v>-0.2965571204976852</v>
       </c>
       <c r="S11" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>251456</v>
+        <v>251225</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D12" t="n">
-        <v>147.5245901639344</v>
+        <v>0</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -1307,21 +1311,21 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>2025-05-08 07:25:00</t>
+          <t>2025-05-08 07:19:00</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>2025-05-08 07:25:00</t>
+          <t>2025-05-08 07:19:00</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>2025-05-08 09:52:31</t>
+          <t>2025-05-08 07:19:00</t>
         </is>
       </c>
       <c r="I12" t="n">
-        <v>8999</v>
+        <v>0</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
@@ -1330,17 +1334,17 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
         </is>
       </c>
       <c r="L12" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M12" t="n">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="N12" t="n">
-        <v>39746</v>
+        <v>39747</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
@@ -1348,15 +1352,15 @@
         </is>
       </c>
       <c r="P12" t="n">
-        <v>39746</v>
+        <v>39747</v>
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>2025-05-09 00:00:00</t>
+          <t>2025-04-30 00:00:00</t>
         </is>
       </c>
       <c r="R12" s="1" t="n">
-        <v>-2.411475409837963</v>
+        <v>-0.3048611111111111</v>
       </c>
       <c r="S12" t="n">
         <v>1</v>
@@ -1364,41 +1368,41 @@
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>251840</v>
+        <v>251547</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C13" t="n">
         <v>30</v>
       </c>
       <c r="D13" t="n">
-        <v>93.67213114754098</v>
+        <v>184.9154929577465</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>2025-05-08 09:52:31</t>
+          <t>2025-05-08 07:19:00</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>2025-05-08 10:22:31</t>
+          <t>2025-05-08 07:49:00</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>2025-05-08 10:22:31</t>
+          <t>2025-05-08 07:49:00</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>2025-05-08 11:56:11</t>
+          <t>2025-05-08 10:53:54</t>
         </is>
       </c>
       <c r="I13" t="n">
-        <v>5714</v>
+        <v>13129</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
@@ -1411,13 +1415,13 @@
         </is>
       </c>
       <c r="L13" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M13" t="n">
         <v>70</v>
       </c>
       <c r="N13" t="n">
-        <v>39758</v>
+        <v>39749</v>
       </c>
       <c r="O13" t="inlineStr">
         <is>
@@ -1425,57 +1429,57 @@
         </is>
       </c>
       <c r="P13" t="n">
-        <v>39758</v>
+        <v>39749</v>
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>2025-05-09 00:00:00</t>
+          <t>2025-05-06 00:00:00</t>
         </is>
       </c>
       <c r="R13" s="1" t="n">
-        <v>-0.4973588342476852</v>
+        <v>-1.454107981215278</v>
       </c>
       <c r="S13" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>251229</v>
+        <v>250759</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D14" t="n">
-        <v>307.1967213114754</v>
+        <v>118.2816901408451</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>2025-05-08 11:56:11</t>
+          <t>2025-05-08 10:53:54</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>2025-05-08 12:21:11</t>
+          <t>2025-05-08 11:23:54</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>2025-05-08 12:21:11</t>
+          <t>2025-05-08 11:23:54</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>2025-05-09 09:28:23</t>
+          <t>2025-05-08 13:22:11</t>
         </is>
       </c>
       <c r="I14" t="n">
-        <v>18739</v>
+        <v>8398</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
@@ -1484,19 +1488,17 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12</t>
         </is>
       </c>
       <c r="L14" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="M14" t="n">
-        <v>70</v>
-      </c>
-      <c r="N14" t="inlineStr">
-        <is>
-          <t>39723 (esterno)</t>
-        </is>
+        <v>76</v>
+      </c>
+      <c r="N14" t="n">
+        <v>39747</v>
       </c>
       <c r="O14" t="inlineStr">
         <is>
@@ -1504,15 +1506,15 @@
         </is>
       </c>
       <c r="P14" t="n">
-        <v>39723</v>
+        <v>39747</v>
       </c>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>2025-05-15 00:00:00</t>
+          <t>2025-03-13 00:00:00</t>
         </is>
       </c>
       <c r="R14" s="1" t="n">
-        <v>0</v>
+        <v>-0.5570813771527778</v>
       </c>
       <c r="S14" t="n">
         <v>1</v>
@@ -1520,41 +1522,41 @@
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>251782</v>
+        <v>250894</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>R12</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C15" t="n">
         <v>17</v>
       </c>
       <c r="D15" t="n">
-        <v>170.0422535211268</v>
+        <v>623.4084507042254</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>2025-05-08 12:00:00</t>
+          <t>2025-05-08 13:22:11</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>2025-05-08 12:17:00</t>
+          <t>2025-05-08 13:39:11</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>2025-05-08 12:17:00</t>
+          <t>2025-05-08 13:39:11</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>2025-05-09 07:07:02</t>
+          <t>2025-05-12 08:02:36</t>
         </is>
       </c>
       <c r="I15" t="n">
-        <v>12073</v>
+        <v>44262</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
@@ -1563,36 +1565,34 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L15" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="M15" t="n">
         <v>76</v>
       </c>
       <c r="N15" t="n">
-        <v>39754</v>
-      </c>
-      <c r="O15" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
+        <v>39755</v>
+      </c>
+      <c r="O15" t="n">
+        <v>0</v>
       </c>
       <c r="P15" t="n">
-        <v>39754</v>
+        <v>0</v>
       </c>
       <c r="Q15" t="inlineStr">
         <is>
-          <t>2025-05-16 00:00:00</t>
+          <t>2025-05-05 00:00:00</t>
         </is>
       </c>
       <c r="R15" s="1" t="n">
-        <v>-0.2965571204976852</v>
+        <v>0</v>
       </c>
       <c r="S15" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16">
@@ -1672,41 +1672,41 @@
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>251416</v>
+        <v>251227</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>R3</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D17" t="n">
-        <v>229.0204081632653</v>
+        <v>0</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>2025-05-08 07:00:00</t>
+          <t>2025-05-07 07:00:00</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>2025-05-08 07:35:00</t>
+          <t>2025-05-07 07:34:00</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>2025-05-08 07:35:00</t>
+          <t>2025-05-07 07:34:00</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>2025-05-08 11:24:01</t>
+          <t>2025-05-07 07:34:00</t>
         </is>
       </c>
       <c r="I17" t="n">
-        <v>11222</v>
+        <v>0</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
@@ -1715,39 +1715,41 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
         </is>
       </c>
       <c r="L17" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M17" t="n">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="N17" t="n">
-        <v>39755</v>
-      </c>
-      <c r="O17" t="n">
-        <v>0</v>
+        <v>39746</v>
+      </c>
+      <c r="O17" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
       </c>
       <c r="P17" t="n">
-        <v>0</v>
+        <v>39746</v>
       </c>
       <c r="Q17" t="inlineStr">
         <is>
-          <t>2025-04-23 00:00:00</t>
+          <t>2025-05-05 00:00:00</t>
         </is>
       </c>
       <c r="R17" s="1" t="n">
-        <v>0</v>
+        <v>-1.315277777777778</v>
       </c>
       <c r="S17" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>251742</v>
+        <v>251455</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
@@ -1755,33 +1757,33 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="D18" t="n">
-        <v>128.53125</v>
+        <v>82.765625</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>2025-05-07 07:00:00</t>
+          <t>2025-05-07 07:34:00</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>2025-05-07 07:19:00</t>
+          <t>2025-05-07 08:04:00</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>2025-05-07 07:19:00</t>
+          <t>2025-05-07 08:04:00</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>2025-05-07 09:27:31</t>
+          <t>2025-05-07 09:26:45</t>
         </is>
       </c>
       <c r="I18" t="n">
-        <v>8226</v>
+        <v>5297</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
@@ -1812,11 +1814,11 @@
       </c>
       <c r="Q18" t="inlineStr">
         <is>
-          <t>2025-05-15 00:00:00</t>
+          <t>2025-04-15 00:00:00</t>
         </is>
       </c>
       <c r="R18" s="1" t="n">
-        <v>-0.3941189236111111</v>
+        <v>-0.3935872395833334</v>
       </c>
       <c r="S18" t="n">
         <v>7</v>
@@ -1824,7 +1826,7 @@
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>251455</v>
+        <v>251391</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
@@ -1832,33 +1834,33 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D19" t="n">
-        <v>82.765625</v>
+        <v>91.640625</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>2025-05-07 09:27:31</t>
+          <t>2025-05-07 09:26:45</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>2025-05-07 09:42:31</t>
+          <t>2025-05-07 09:43:45</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>2025-05-07 09:42:31</t>
+          <t>2025-05-07 09:43:45</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>2025-05-07 11:05:17</t>
+          <t>2025-05-07 11:15:24</t>
         </is>
       </c>
       <c r="I19" t="n">
-        <v>5297</v>
+        <v>5865</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
@@ -1871,7 +1873,7 @@
         </is>
       </c>
       <c r="L19" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M19" t="n">
         <v>70</v>
@@ -1889,11 +1891,11 @@
       </c>
       <c r="Q19" t="inlineStr">
         <is>
-          <t>2025-04-15 00:00:00</t>
+          <t>2025-04-23 00:00:00</t>
         </is>
       </c>
       <c r="R19" s="1" t="n">
-        <v>-0.46201171875</v>
+        <v>-0.4690321180555556</v>
       </c>
       <c r="S19" t="n">
         <v>7</v>
@@ -1901,7 +1903,7 @@
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>251391</v>
+        <v>251395</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
@@ -1912,30 +1914,30 @@
         <v>17</v>
       </c>
       <c r="D20" t="n">
-        <v>91.640625</v>
+        <v>35.34375</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>2025-05-07 11:05:17</t>
+          <t>2025-05-07 11:15:24</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>2025-05-07 11:22:17</t>
+          <t>2025-05-07 11:32:24</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>2025-05-07 11:22:17</t>
+          <t>2025-05-07 11:32:24</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>2025-05-07 12:53:56</t>
+          <t>2025-05-07 12:07:45</t>
         </is>
       </c>
       <c r="I20" t="n">
-        <v>5865</v>
+        <v>2262</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
@@ -1948,7 +1950,7 @@
         </is>
       </c>
       <c r="L20" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M20" t="n">
         <v>70</v>
@@ -1970,7 +1972,7 @@
         </is>
       </c>
       <c r="R20" s="1" t="n">
-        <v>-0.5374565972222223</v>
+        <v>-0.5053819444444444</v>
       </c>
       <c r="S20" t="n">
         <v>7</v>
@@ -1978,7 +1980,7 @@
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>251395</v>
+        <v>251371</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
@@ -1986,33 +1988,33 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D21" t="n">
-        <v>35.34375</v>
+        <v>0</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>2025-05-07 12:53:56</t>
+          <t>2025-05-07 12:07:45</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>2025-05-07 13:10:56</t>
+          <t>2025-05-07 12:26:45</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>2025-05-07 13:10:56</t>
+          <t>2025-05-07 12:26:45</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>2025-05-07 13:46:16</t>
+          <t>2025-05-07 12:26:45</t>
         </is>
       </c>
       <c r="I21" t="n">
-        <v>2262</v>
+        <v>0</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
@@ -2025,13 +2027,15 @@
         </is>
       </c>
       <c r="L21" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="M21" t="n">
         <v>70</v>
       </c>
-      <c r="N21" t="n">
-        <v>39749</v>
+      <c r="N21" t="inlineStr">
+        <is>
+          <t>39666 (esterno)</t>
+        </is>
       </c>
       <c r="O21" t="inlineStr">
         <is>
@@ -2039,15 +2043,15 @@
         </is>
       </c>
       <c r="P21" t="n">
-        <v>39749</v>
+        <v>39666</v>
       </c>
       <c r="Q21" t="inlineStr">
         <is>
-          <t>2025-04-23 00:00:00</t>
+          <t>2025-04-24 00:00:00</t>
         </is>
       </c>
       <c r="R21" s="1" t="n">
-        <v>-0.5738064236111111</v>
+        <v>-13.51857638888889</v>
       </c>
       <c r="S21" t="n">
         <v>7</v>
@@ -2055,7 +2059,7 @@
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>251371</v>
+        <v>251396</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
@@ -2066,30 +2070,30 @@
         <v>19</v>
       </c>
       <c r="D22" t="n">
-        <v>0</v>
+        <v>35.34375</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>2025-05-07 13:46:16</t>
+          <t>2025-05-07 12:26:45</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>2025-05-07 14:05:16</t>
+          <t>2025-05-07 12:45:45</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>2025-05-07 14:05:16</t>
+          <t>2025-05-07 12:45:45</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>2025-05-07 14:05:16</t>
+          <t>2025-05-07 13:21:05</t>
         </is>
       </c>
       <c r="I22" t="n">
-        <v>0</v>
+        <v>2262</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
@@ -2102,15 +2106,13 @@
         </is>
       </c>
       <c r="L22" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M22" t="n">
         <v>70</v>
       </c>
-      <c r="N22" t="inlineStr">
-        <is>
-          <t>39666 (esterno)</t>
-        </is>
+      <c r="N22" t="n">
+        <v>39749</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
@@ -2118,15 +2120,15 @@
         </is>
       </c>
       <c r="P22" t="n">
-        <v>39666</v>
+        <v>39749</v>
       </c>
       <c r="Q22" t="inlineStr">
         <is>
-          <t>2025-04-24 00:00:00</t>
+          <t>2025-05-02 00:00:00</t>
         </is>
       </c>
       <c r="R22" s="1" t="n">
-        <v>-13.58700086805556</v>
+        <v>-0.5563151041666666</v>
       </c>
       <c r="S22" t="n">
         <v>7</v>
@@ -2134,7 +2136,7 @@
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>251396</v>
+        <v>251548</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
@@ -2145,30 +2147,30 @@
         <v>19</v>
       </c>
       <c r="D23" t="n">
-        <v>35.34375</v>
+        <v>206.90625</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>2025-05-07 14:05:16</t>
+          <t>2025-05-07 13:21:05</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>2025-05-07 14:24:16</t>
+          <t>2025-05-07 13:40:05</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>2025-05-07 14:24:16</t>
+          <t>2025-05-07 13:40:05</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>2025-05-07 14:59:37</t>
+          <t>2025-05-08 09:07:00</t>
         </is>
       </c>
       <c r="I23" t="n">
-        <v>2262</v>
+        <v>13242</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
@@ -2181,7 +2183,7 @@
         </is>
       </c>
       <c r="L23" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="M23" t="n">
         <v>70</v>
@@ -2199,11 +2201,11 @@
       </c>
       <c r="Q23" t="inlineStr">
         <is>
-          <t>2025-05-02 00:00:00</t>
+          <t>2025-05-06 00:00:00</t>
         </is>
       </c>
       <c r="R23" s="1" t="n">
-        <v>-0.6247395833333333</v>
+        <v>-1.379861111111111</v>
       </c>
       <c r="S23" t="n">
         <v>7</v>
@@ -2211,7 +2213,7 @@
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>251548</v>
+        <v>250923</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
@@ -2219,33 +2221,33 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="D24" t="n">
-        <v>206.90625</v>
+        <v>109.46875</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>2025-05-07 14:59:37</t>
+          <t>2025-05-08 09:07:00</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>2025-05-08 07:18:37</t>
+          <t>2025-05-08 09:39:00</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>2025-05-08 07:18:37</t>
+          <t>2025-05-08 09:39:00</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>2025-05-08 10:45:31</t>
+          <t>2025-05-08 11:28:28</t>
         </is>
       </c>
       <c r="I24" t="n">
-        <v>13242</v>
+        <v>7006</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
@@ -2254,14 +2256,14 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
         </is>
       </c>
       <c r="L24" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M24" t="n">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="N24" t="n">
         <v>39749</v>
@@ -2276,19 +2278,19 @@
       </c>
       <c r="Q24" t="inlineStr">
         <is>
-          <t>2025-05-06 00:00:00</t>
+          <t>2025-04-07 00:00:00</t>
         </is>
       </c>
       <c r="R24" s="1" t="n">
-        <v>-1.448285590277778</v>
+        <v>-1.478103298611111</v>
       </c>
       <c r="S24" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>250923</v>
+        <v>251477</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
@@ -2296,33 +2298,33 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="D25" t="n">
-        <v>109.46875</v>
+        <v>468.734375</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>2025-05-08 10:45:31</t>
+          <t>2025-05-08 11:28:28</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>2025-05-08 11:17:31</t>
+          <t>2025-05-08 11:47:28</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>2025-05-08 11:17:31</t>
+          <t>2025-05-08 11:47:28</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>2025-05-08 13:07:00</t>
+          <t>2025-05-09 11:36:12</t>
         </is>
       </c>
       <c r="I25" t="n">
-        <v>7006</v>
+        <v>29999</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
@@ -2331,17 +2333,17 @@
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L25" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="M25" t="n">
         <v>76</v>
       </c>
       <c r="N25" t="n">
-        <v>39749</v>
+        <v>39760</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
@@ -2349,57 +2351,57 @@
         </is>
       </c>
       <c r="P25" t="n">
-        <v>39749</v>
+        <v>39760</v>
       </c>
       <c r="Q25" t="inlineStr">
         <is>
-          <t>2025-04-07 00:00:00</t>
+          <t>2025-04-28 00:00:00</t>
         </is>
       </c>
       <c r="R25" s="1" t="n">
-        <v>-1.546527777777778</v>
+        <v>-2.483474392361111</v>
       </c>
       <c r="S25" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>251477</v>
+        <v>251456</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>R3</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>19</v>
+        <v>40</v>
       </c>
       <c r="D26" t="n">
-        <v>468.734375</v>
+        <v>183.6530612244898</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>2025-05-08 13:07:00</t>
+          <t>2025-05-08 07:00:00</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>2025-05-08 13:26:00</t>
+          <t>2025-05-08 07:40:00</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>2025-05-08 13:26:00</t>
+          <t>2025-05-08 07:40:00</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>2025-05-09 13:14:44</t>
+          <t>2025-05-08 10:43:39</t>
         </is>
       </c>
       <c r="I26" t="n">
-        <v>29999</v>
+        <v>8999</v>
       </c>
       <c r="J26" t="inlineStr">
         <is>
@@ -2408,17 +2410,17 @@
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L26" t="n">
         <v>3</v>
       </c>
       <c r="M26" t="n">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="N26" t="n">
-        <v>39760</v>
+        <v>39746</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
@@ -2426,15 +2428,15 @@
         </is>
       </c>
       <c r="P26" t="n">
-        <v>39760</v>
+        <v>39746</v>
       </c>
       <c r="Q26" t="inlineStr">
         <is>
-          <t>2025-04-28 00:00:00</t>
+          <t>2025-05-09 00:00:00</t>
         </is>
       </c>
       <c r="R26" s="1" t="n">
-        <v>-2.551898871527778</v>
+        <v>-2.446981292511574</v>
       </c>
       <c r="S26" t="n">
         <v>1</v>
@@ -2442,41 +2444,41 @@
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>251284</v>
+        <v>251416</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>CASON</t>
+          <t>R3</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>40.5</v>
+        <v>40</v>
       </c>
       <c r="D27" t="n">
-        <v>297.0909090909091</v>
+        <v>229.0204081632653</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>2025-05-09 07:00:00</t>
+          <t>2025-05-08 10:43:39</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>2025-05-09 07:40:30</t>
+          <t>2025-05-08 11:23:39</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>2025-05-09 07:40:30</t>
+          <t>2025-05-08 11:23:39</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>2025-05-09 12:37:35</t>
+          <t>2025-05-09 07:12:40</t>
         </is>
       </c>
       <c r="I27" t="n">
-        <v>16340</v>
+        <v>11222</v>
       </c>
       <c r="J27" t="inlineStr">
         <is>
@@ -2485,36 +2487,34 @@
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>CASON ;R6</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L27" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="M27" t="n">
         <v>70</v>
       </c>
       <c r="N27" t="n">
-        <v>39747</v>
-      </c>
-      <c r="O27" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
+        <v>39755</v>
+      </c>
+      <c r="O27" t="n">
+        <v>0</v>
       </c>
       <c r="P27" t="n">
-        <v>39747</v>
+        <v>0</v>
       </c>
       <c r="Q27" t="inlineStr">
         <is>
-          <t>2025-05-12 00:00:00</t>
+          <t>2025-04-23 00:00:00</t>
         </is>
       </c>
       <c r="R27" s="1" t="n">
-        <v>-1.526104797974537</v>
+        <v>0</v>
       </c>
       <c r="S27" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Rotta direi solo LS3 con alfa = 0 in caso di sequenzialità con LS2
</commit_message>
<xml_diff>
--- a/PS-VRP/Dati_output/insert_inter.xlsx
+++ b/PS-VRP/Dati_output/insert_inter.xlsx
@@ -515,62 +515,60 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>251706</v>
+        <v>251225</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>T3</t>
+          <t>R12</t>
         </is>
       </c>
       <c r="C2" t="n">
+        <v>19</v>
+      </c>
+      <c r="D2" t="n">
         <v>0</v>
       </c>
-      <c r="D2" t="n">
-        <v>50.79365079365079</v>
-      </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2025-05-12 07:00:00</t>
+          <t>2025-05-08 12:00:00</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2025-05-12 07:00:00</t>
+          <t>2025-05-08 12:19:00</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>2025-05-12 07:00:00</t>
+          <t>2025-05-08 12:19:00</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>2025-05-12 07:50:47</t>
+          <t>2025-05-08 12:19:00</t>
         </is>
       </c>
       <c r="I2" t="n">
-        <v>3200</v>
+        <v>0</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>foglio</t>
+          <t>bobina</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>T3</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
         </is>
       </c>
       <c r="L2" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="M2" t="n">
-        <v>0</v>
-      </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>39764 (esterno)</t>
-        </is>
+        <v>76</v>
+      </c>
+      <c r="N2" t="n">
+        <v>39747</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
@@ -578,53 +576,53 @@
         </is>
       </c>
       <c r="P2" t="n">
-        <v>39764</v>
+        <v>39747</v>
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>2025-05-14 00:00:00</t>
+          <t>2025-04-30 00:00:00</t>
         </is>
       </c>
       <c r="R2" s="1" t="n">
-        <v>0</v>
+        <v>-0.5131944444444444</v>
       </c>
       <c r="S2" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>251050</v>
+        <v>251227</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>R12</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>217</v>
+        <v>15</v>
       </c>
       <c r="D3" t="n">
         <v>0</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2025-05-09 07:00:00</t>
+          <t>2025-05-08 12:19:00</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2025-05-09 10:37:00</t>
+          <t>2025-05-08 12:34:00</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>2025-05-09 10:37:00</t>
+          <t>2025-05-08 12:34:00</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>2025-05-09 10:37:00</t>
+          <t>2025-05-08 12:34:00</t>
         </is>
       </c>
       <c r="I3" t="n">
@@ -637,17 +635,17 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
         </is>
       </c>
       <c r="L3" t="n">
-        <v>38</v>
+        <v>4</v>
       </c>
       <c r="M3" t="n">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="N3" t="n">
-        <v>39747</v>
+        <v>39746</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
@@ -655,57 +653,57 @@
         </is>
       </c>
       <c r="P3" t="n">
-        <v>39747</v>
+        <v>39746</v>
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>2025-04-16 00:00:00</t>
+          <t>2025-05-05 00:00:00</t>
         </is>
       </c>
       <c r="R3" s="1" t="n">
-        <v>-1.442361111111111</v>
+        <v>-2.523611111111111</v>
       </c>
       <c r="S3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>251054</v>
+        <v>250923</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>R12</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>98.67605633802818</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2025-05-09 10:37:00</t>
+          <t>2025-05-08 12:34:00</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>2025-05-09 11:12:00</t>
+          <t>2025-05-08 12:51:00</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>2025-05-09 11:12:00</t>
+          <t>2025-05-08 12:51:00</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>2025-05-09 11:12:00</t>
+          <t>2025-05-08 14:29:40</t>
         </is>
       </c>
       <c r="I4" t="n">
-        <v>0</v>
+        <v>7006</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
@@ -714,17 +712,17 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
         </is>
       </c>
       <c r="L4" t="n">
-        <v>38</v>
+        <v>5</v>
       </c>
       <c r="M4" t="n">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="N4" t="n">
-        <v>39747</v>
+        <v>39749</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
@@ -732,15 +730,15 @@
         </is>
       </c>
       <c r="P4" t="n">
-        <v>39747</v>
+        <v>39749</v>
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>2025-04-16 00:00:00</t>
+          <t>2025-04-07 00:00:00</t>
         </is>
       </c>
       <c r="R4" s="1" t="n">
-        <v>-1.466666666666667</v>
+        <v>-1.603941705787037</v>
       </c>
       <c r="S4" t="n">
         <v>2</v>
@@ -748,41 +746,41 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>251081</v>
+        <v>250894</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>R12</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>125</v>
+        <v>15</v>
       </c>
       <c r="D5" t="n">
-        <v>42.42253521126761</v>
+        <v>623.4084507042254</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2025-05-09 11:12:00</t>
+          <t>2025-05-08 14:29:40</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>2025-05-09 13:17:00</t>
+          <t>2025-05-08 14:44:40</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>2025-05-09 13:17:00</t>
+          <t>2025-05-08 14:44:40</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>2025-05-09 13:59:25</t>
+          <t>2025-05-12 09:08:05</t>
         </is>
       </c>
       <c r="I5" t="n">
-        <v>3012</v>
+        <v>44262</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
@@ -791,154 +789,152 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L5" t="n">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="M5" t="n">
-        <v>70</v>
-      </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>39750 (esterno)</t>
-        </is>
-      </c>
-      <c r="O5" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
+        <v>76</v>
+      </c>
+      <c r="N5" t="n">
+        <v>39755</v>
+      </c>
+      <c r="O5" t="n">
+        <v>0</v>
       </c>
       <c r="P5" t="n">
-        <v>39750</v>
+        <v>0</v>
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>2025-04-23 00:00:00</t>
+          <t>2025-05-05 00:00:00</t>
         </is>
       </c>
       <c r="R5" s="1" t="n">
-        <v>-16.58293231612268</v>
+        <v>0</v>
       </c>
       <c r="S5" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>251284</v>
+        <v>251706</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>CASON</t>
+          <t>T3</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>40.5</v>
+        <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>297.0909090909091</v>
+        <v>50.79365079365079</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2025-05-09 07:00:00</t>
+          <t>2025-05-12 07:00:00</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2025-05-09 07:40:30</t>
+          <t>2025-05-12 07:00:00</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>2025-05-09 07:40:30</t>
+          <t>2025-05-12 07:00:00</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>2025-05-09 12:37:35</t>
+          <t>2025-05-12 07:50:47</t>
         </is>
       </c>
       <c r="I6" t="n">
-        <v>16340</v>
+        <v>3200</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>bobina</t>
+          <t>foglio</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>CASON ;R6</t>
+          <t>T3</t>
         </is>
       </c>
       <c r="L6" t="n">
+        <v>0</v>
+      </c>
+      <c r="M6" t="n">
+        <v>0</v>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>39764 (esterno)</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="P6" t="n">
+        <v>39764</v>
+      </c>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>2025-05-14 00:00:00</t>
+        </is>
+      </c>
+      <c r="R6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="S6" t="n">
         <v>7</v>
-      </c>
-      <c r="M6" t="n">
-        <v>70</v>
-      </c>
-      <c r="N6" t="n">
-        <v>39747</v>
-      </c>
-      <c r="O6" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="P6" t="n">
-        <v>39747</v>
-      </c>
-      <c r="Q6" t="inlineStr">
-        <is>
-          <t>2025-05-12 00:00:00</t>
-        </is>
-      </c>
-      <c r="R6" s="1" t="n">
-        <v>-1.526104797974537</v>
-      </c>
-      <c r="S6" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>251742</v>
+        <v>251164</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>30</v>
+        <v>57</v>
       </c>
       <c r="D7" t="n">
-        <v>134.8524590163935</v>
+        <v>140.8450704225352</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2025-05-08 07:00:00</t>
+          <t>2025-05-09 07:00:00</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>2025-05-08 07:30:00</t>
+          <t>2025-05-09 07:57:00</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>2025-05-08 07:30:00</t>
+          <t>2025-05-09 07:57:00</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>2025-05-08 09:44:51</t>
+          <t>2025-05-09 10:17:50</t>
         </is>
       </c>
       <c r="I7" t="n">
-        <v>8226</v>
+        <v>10000</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
@@ -951,7 +947,7 @@
         </is>
       </c>
       <c r="L7" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M7" t="n">
         <v>70</v>
@@ -969,53 +965,53 @@
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>2025-05-15 00:00:00</t>
+          <t>2025-04-22 00:00:00</t>
         </is>
       </c>
       <c r="R7" s="1" t="n">
-        <v>-1.406147540983796</v>
+        <v>-2.429059076678241</v>
       </c>
       <c r="S7" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>251164</v>
+        <v>251050</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>30</v>
+        <v>195</v>
       </c>
       <c r="D8" t="n">
-        <v>163.9344262295082</v>
+        <v>0</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2025-05-08 09:44:51</t>
+          <t>2025-05-09 10:17:50</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>2025-05-08 10:14:51</t>
+          <t>2025-05-09 13:32:50</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>2025-05-08 10:14:51</t>
+          <t>2025-05-09 13:32:50</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>2025-05-08 12:58:47</t>
+          <t>2025-05-09 13:32:50</t>
         </is>
       </c>
       <c r="I8" t="n">
-        <v>10000</v>
+        <v>0</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
@@ -1024,17 +1020,17 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="L8" t="n">
-        <v>6</v>
+        <v>38</v>
       </c>
       <c r="M8" t="n">
         <v>70</v>
       </c>
       <c r="N8" t="n">
-        <v>39749</v>
+        <v>39747</v>
       </c>
       <c r="O8" t="inlineStr">
         <is>
@@ -1042,57 +1038,57 @@
         </is>
       </c>
       <c r="P8" t="n">
-        <v>39749</v>
+        <v>39747</v>
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>2025-04-22 00:00:00</t>
+          <t>2025-04-16 00:00:00</t>
         </is>
       </c>
       <c r="R8" s="1" t="n">
-        <v>-1.540824225868056</v>
+        <v>-1.564475743344907</v>
       </c>
       <c r="S8" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>251840</v>
+        <v>251054</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="D9" t="n">
-        <v>93.67213114754098</v>
+        <v>0</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>2025-05-08 12:58:47</t>
+          <t>2025-05-09 13:32:50</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>2025-05-08 13:23:47</t>
+          <t>2025-05-09 14:07:50</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>2025-05-08 13:23:47</t>
+          <t>2025-05-09 14:07:50</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>2025-05-08 14:57:27</t>
+          <t>2025-05-09 14:07:50</t>
         </is>
       </c>
       <c r="I9" t="n">
-        <v>5714</v>
+        <v>0</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
@@ -1101,17 +1097,17 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="L9" t="n">
-        <v>5</v>
+        <v>38</v>
       </c>
       <c r="M9" t="n">
         <v>70</v>
       </c>
       <c r="N9" t="n">
-        <v>39758</v>
+        <v>39747</v>
       </c>
       <c r="O9" t="inlineStr">
         <is>
@@ -1119,57 +1115,57 @@
         </is>
       </c>
       <c r="P9" t="n">
-        <v>39758</v>
+        <v>39747</v>
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>2025-05-09 00:00:00</t>
+          <t>2025-04-16 00:00:00</t>
         </is>
       </c>
       <c r="R9" s="1" t="n">
-        <v>-0.6232354280555555</v>
+        <v>-1.588781298900463</v>
       </c>
       <c r="S9" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>251229</v>
+        <v>251081</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>25</v>
+        <v>125</v>
       </c>
       <c r="D10" t="n">
-        <v>307.1967213114754</v>
+        <v>42.42253521126761</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2025-05-08 14:57:27</t>
+          <t>2025-05-09 14:07:50</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>2025-05-09 07:22:27</t>
+          <t>2025-05-12 08:12:50</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>2025-05-09 07:22:27</t>
+          <t>2025-05-12 08:12:50</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>2025-05-09 12:29:39</t>
+          <t>2025-05-12 08:55:16</t>
         </is>
       </c>
       <c r="I10" t="n">
-        <v>18739</v>
+        <v>3012</v>
       </c>
       <c r="J10" t="inlineStr">
         <is>
@@ -1178,18 +1174,18 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R9</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="L10" t="n">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="M10" t="n">
         <v>70</v>
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>39723 (esterno)</t>
+          <t>39750 (esterno)</t>
         </is>
       </c>
       <c r="O10" t="inlineStr">
@@ -1198,57 +1194,57 @@
         </is>
       </c>
       <c r="P10" t="n">
-        <v>39723</v>
+        <v>39750</v>
       </c>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>2025-05-15 00:00:00</t>
+          <t>2025-04-23 00:00:00</t>
         </is>
       </c>
       <c r="R10" s="1" t="n">
-        <v>0</v>
+        <v>-19.37171361502315</v>
       </c>
       <c r="S10" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>251782</v>
+        <v>251284</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>R12</t>
+          <t>CASON</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>17</v>
+        <v>40.5</v>
       </c>
       <c r="D11" t="n">
-        <v>170.0422535211268</v>
+        <v>297.0909090909091</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>2025-05-08 12:00:00</t>
+          <t>2025-05-09 07:00:00</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>2025-05-08 12:17:00</t>
+          <t>2025-05-09 07:40:30</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>2025-05-08 12:17:00</t>
+          <t>2025-05-09 07:40:30</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>2025-05-09 07:07:02</t>
+          <t>2025-05-09 12:37:35</t>
         </is>
       </c>
       <c r="I11" t="n">
-        <v>12073</v>
+        <v>16340</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
@@ -1257,17 +1253,17 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R6 ;R9</t>
+          <t>CASON ;R6</t>
         </is>
       </c>
       <c r="L11" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="M11" t="n">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="N11" t="n">
-        <v>39754</v>
+        <v>39747</v>
       </c>
       <c r="O11" t="inlineStr">
         <is>
@@ -1275,15 +1271,15 @@
         </is>
       </c>
       <c r="P11" t="n">
-        <v>39754</v>
+        <v>39747</v>
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>2025-05-16 00:00:00</t>
+          <t>2025-05-12 00:00:00</t>
         </is>
       </c>
       <c r="R11" s="1" t="n">
-        <v>-0.2965571204976852</v>
+        <v>-1.526104797974537</v>
       </c>
       <c r="S11" t="n">
         <v>1</v>
@@ -1291,76 +1287,78 @@
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>251225</v>
+        <v>251229</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>BIMEC 5</t>
+          <t>R10</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>19</v>
+        <v>40</v>
       </c>
       <c r="D12" t="n">
+        <v>307.1967213114754</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>2025-05-08 07:00:00</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>2025-05-08 07:40:00</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>2025-05-08 07:40:00</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>2025-05-08 12:47:11</t>
+        </is>
+      </c>
+      <c r="I12" t="n">
+        <v>18739</v>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>bobina</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R9</t>
+        </is>
+      </c>
+      <c r="L12" t="n">
+        <v>6</v>
+      </c>
+      <c r="M12" t="n">
+        <v>70</v>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>39723 (esterno)</t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="P12" t="n">
+        <v>39723</v>
+      </c>
+      <c r="Q12" t="inlineStr">
+        <is>
+          <t>2025-05-15 00:00:00</t>
+        </is>
+      </c>
+      <c r="R12" s="1" t="n">
         <v>0</v>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>2025-05-08 07:00:00</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>2025-05-08 07:19:00</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>2025-05-08 07:19:00</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>2025-05-08 07:19:00</t>
-        </is>
-      </c>
-      <c r="I12" t="n">
-        <v>0</v>
-      </c>
-      <c r="J12" t="inlineStr">
-        <is>
-          <t>bobina</t>
-        </is>
-      </c>
-      <c r="K12" t="inlineStr">
-        <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
-        </is>
-      </c>
-      <c r="L12" t="n">
-        <v>4</v>
-      </c>
-      <c r="M12" t="n">
-        <v>76</v>
-      </c>
-      <c r="N12" t="n">
-        <v>39747</v>
-      </c>
-      <c r="O12" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="P12" t="n">
-        <v>39747</v>
-      </c>
-      <c r="Q12" t="inlineStr">
-        <is>
-          <t>2025-04-30 00:00:00</t>
-        </is>
-      </c>
-      <c r="R12" s="1" t="n">
-        <v>-0.3048611111111111</v>
       </c>
       <c r="S12" t="n">
         <v>1</v>
@@ -1368,41 +1366,41 @@
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>251547</v>
+        <v>251456</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>BIMEC 5</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="D13" t="n">
-        <v>184.9154929577465</v>
+        <v>140.609375</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>2025-05-08 07:19:00</t>
+          <t>2025-05-07 07:00:00</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>2025-05-08 07:49:00</t>
+          <t>2025-05-07 07:17:00</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>2025-05-08 07:49:00</t>
+          <t>2025-05-07 07:17:00</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>2025-05-08 10:53:54</t>
+          <t>2025-05-07 09:37:36</t>
         </is>
       </c>
       <c r="I13" t="n">
-        <v>13129</v>
+        <v>8999</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
@@ -1415,13 +1413,13 @@
         </is>
       </c>
       <c r="L13" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M13" t="n">
         <v>70</v>
       </c>
       <c r="N13" t="n">
-        <v>39749</v>
+        <v>39746</v>
       </c>
       <c r="O13" t="inlineStr">
         <is>
@@ -1429,57 +1427,57 @@
         </is>
       </c>
       <c r="P13" t="n">
-        <v>39749</v>
+        <v>39746</v>
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>2025-05-06 00:00:00</t>
+          <t>2025-05-09 00:00:00</t>
         </is>
       </c>
       <c r="R13" s="1" t="n">
-        <v>-1.454107981215278</v>
+        <v>-1.401117621527778</v>
       </c>
       <c r="S13" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>250759</v>
+        <v>251742</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>BIMEC 5</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="D14" t="n">
-        <v>118.2816901408451</v>
+        <v>128.53125</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>2025-05-08 10:53:54</t>
+          <t>2025-05-07 09:37:36</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>2025-05-08 11:23:54</t>
+          <t>2025-05-07 09:54:36</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>2025-05-08 11:23:54</t>
+          <t>2025-05-07 09:54:36</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>2025-05-08 13:22:11</t>
+          <t>2025-05-07 12:03:08</t>
         </is>
       </c>
       <c r="I14" t="n">
-        <v>8398</v>
+        <v>8226</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
@@ -1488,17 +1486,17 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L14" t="n">
         <v>4</v>
       </c>
       <c r="M14" t="n">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="N14" t="n">
-        <v>39747</v>
+        <v>39749</v>
       </c>
       <c r="O14" t="inlineStr">
         <is>
@@ -1506,57 +1504,57 @@
         </is>
       </c>
       <c r="P14" t="n">
-        <v>39747</v>
+        <v>39749</v>
       </c>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>2025-03-13 00:00:00</t>
+          <t>2025-05-15 00:00:00</t>
         </is>
       </c>
       <c r="R14" s="1" t="n">
-        <v>-0.5570813771527778</v>
+        <v>-0.5021809895833333</v>
       </c>
       <c r="S14" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>250894</v>
+        <v>251455</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>BIMEC 5</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D15" t="n">
-        <v>623.4084507042254</v>
+        <v>82.765625</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>2025-05-08 13:22:11</t>
+          <t>2025-05-07 12:03:08</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>2025-05-08 13:39:11</t>
+          <t>2025-05-07 12:18:08</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>2025-05-08 13:39:11</t>
+          <t>2025-05-07 12:18:08</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>2025-05-12 08:02:36</t>
+          <t>2025-05-07 13:40:54</t>
         </is>
       </c>
       <c r="I15" t="n">
-        <v>44262</v>
+        <v>5297</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
@@ -1565,73 +1563,75 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L15" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M15" t="n">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="N15" t="n">
-        <v>39755</v>
-      </c>
-      <c r="O15" t="n">
-        <v>0</v>
+        <v>39749</v>
+      </c>
+      <c r="O15" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
       </c>
       <c r="P15" t="n">
-        <v>0</v>
+        <v>39749</v>
       </c>
       <c r="Q15" t="inlineStr">
         <is>
-          <t>2025-05-05 00:00:00</t>
+          <t>2025-04-15 00:00:00</t>
         </is>
       </c>
       <c r="R15" s="1" t="n">
-        <v>0</v>
+        <v>-0.5700737847222223</v>
       </c>
       <c r="S15" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>251651</v>
+        <v>251840</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>BIMEC 4</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="D16" t="n">
-        <v>767.7049180327868</v>
+        <v>89.28125</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>2025-05-09 07:00:00</t>
+          <t>2025-05-07 13:40:54</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>2025-05-09 07:29:00</t>
+          <t>2025-05-07 13:57:54</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>2025-05-09 07:29:00</t>
+          <t>2025-05-07 13:57:54</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>2025-05-12 12:16:42</t>
+          <t>2025-05-08 07:27:11</t>
         </is>
       </c>
       <c r="I16" t="n">
-        <v>46830</v>
+        <v>5714</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
@@ -1640,39 +1640,41 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L16" t="n">
         <v>5</v>
       </c>
       <c r="M16" t="n">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="N16" t="n">
-        <v>39755</v>
-      </c>
-      <c r="O16" t="n">
-        <v>0</v>
+        <v>39758</v>
+      </c>
+      <c r="O16" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
       </c>
       <c r="P16" t="n">
-        <v>0</v>
+        <v>39758</v>
       </c>
       <c r="Q16" t="inlineStr">
         <is>
-          <t>2025-05-12 00:00:00</t>
+          <t>2025-05-09 00:00:00</t>
         </is>
       </c>
       <c r="R16" s="1" t="n">
-        <v>0</v>
+        <v>-0.310546875</v>
       </c>
       <c r="S16" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>251227</v>
+        <v>251391</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
@@ -1680,33 +1682,33 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="D17" t="n">
-        <v>0</v>
+        <v>91.640625</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>2025-05-07 07:00:00</t>
+          <t>2025-05-08 07:27:11</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>2025-05-07 07:34:00</t>
+          <t>2025-05-08 07:42:11</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>2025-05-07 07:34:00</t>
+          <t>2025-05-08 07:42:11</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>2025-05-07 07:34:00</t>
+          <t>2025-05-08 09:13:49</t>
         </is>
       </c>
       <c r="I17" t="n">
-        <v>0</v>
+        <v>5865</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
@@ -1715,17 +1717,17 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L17" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M17" t="n">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="N17" t="n">
-        <v>39746</v>
+        <v>39749</v>
       </c>
       <c r="O17" t="inlineStr">
         <is>
@@ -1733,23 +1735,23 @@
         </is>
       </c>
       <c r="P17" t="n">
-        <v>39746</v>
+        <v>39749</v>
       </c>
       <c r="Q17" t="inlineStr">
         <is>
-          <t>2025-05-05 00:00:00</t>
+          <t>2025-04-23 00:00:00</t>
         </is>
       </c>
       <c r="R17" s="1" t="n">
-        <v>-1.315277777777778</v>
+        <v>-1.384602864583333</v>
       </c>
       <c r="S17" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>251455</v>
+        <v>251395</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
@@ -1757,33 +1759,33 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="D18" t="n">
-        <v>82.765625</v>
+        <v>35.34375</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>2025-05-07 07:34:00</t>
+          <t>2025-05-08 09:13:49</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>2025-05-07 08:04:00</t>
+          <t>2025-05-08 09:30:49</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>2025-05-07 08:04:00</t>
+          <t>2025-05-08 09:30:49</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>2025-05-07 09:26:45</t>
+          <t>2025-05-08 10:06:10</t>
         </is>
       </c>
       <c r="I18" t="n">
-        <v>5297</v>
+        <v>2262</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
@@ -1796,7 +1798,7 @@
         </is>
       </c>
       <c r="L18" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M18" t="n">
         <v>70</v>
@@ -1814,11 +1816,11 @@
       </c>
       <c r="Q18" t="inlineStr">
         <is>
-          <t>2025-04-15 00:00:00</t>
+          <t>2025-04-23 00:00:00</t>
         </is>
       </c>
       <c r="R18" s="1" t="n">
-        <v>-0.3935872395833334</v>
+        <v>-1.420952690972222</v>
       </c>
       <c r="S18" t="n">
         <v>7</v>
@@ -1826,7 +1828,7 @@
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>251391</v>
+        <v>251396</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
@@ -1834,33 +1836,33 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D19" t="n">
-        <v>91.640625</v>
+        <v>35.34375</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>2025-05-07 09:26:45</t>
+          <t>2025-05-08 10:06:10</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>2025-05-07 09:43:45</t>
+          <t>2025-05-08 10:21:10</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>2025-05-07 09:43:45</t>
+          <t>2025-05-08 10:21:10</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>2025-05-07 11:15:24</t>
+          <t>2025-05-08 10:56:30</t>
         </is>
       </c>
       <c r="I19" t="n">
-        <v>5865</v>
+        <v>2262</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
@@ -1873,7 +1875,7 @@
         </is>
       </c>
       <c r="L19" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M19" t="n">
         <v>70</v>
@@ -1891,11 +1893,11 @@
       </c>
       <c r="Q19" t="inlineStr">
         <is>
-          <t>2025-04-23 00:00:00</t>
+          <t>2025-05-02 00:00:00</t>
         </is>
       </c>
       <c r="R19" s="1" t="n">
-        <v>-0.4690321180555556</v>
+        <v>-1.455913628472222</v>
       </c>
       <c r="S19" t="n">
         <v>7</v>
@@ -1903,7 +1905,7 @@
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>251395</v>
+        <v>251548</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
@@ -1911,33 +1913,33 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D20" t="n">
-        <v>35.34375</v>
+        <v>206.90625</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>2025-05-07 11:15:24</t>
+          <t>2025-05-08 10:56:30</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>2025-05-07 11:32:24</t>
+          <t>2025-05-08 11:15:30</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>2025-05-07 11:32:24</t>
+          <t>2025-05-08 11:15:30</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>2025-05-07 12:07:45</t>
+          <t>2025-05-08 14:42:25</t>
         </is>
       </c>
       <c r="I20" t="n">
-        <v>2262</v>
+        <v>13242</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
@@ -1950,7 +1952,7 @@
         </is>
       </c>
       <c r="L20" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="M20" t="n">
         <v>70</v>
@@ -1968,11 +1970,11 @@
       </c>
       <c r="Q20" t="inlineStr">
         <is>
-          <t>2025-04-23 00:00:00</t>
+          <t>2025-05-06 00:00:00</t>
         </is>
       </c>
       <c r="R20" s="1" t="n">
-        <v>-0.5053819444444444</v>
+        <v>-1.61279296875</v>
       </c>
       <c r="S20" t="n">
         <v>7</v>
@@ -1980,7 +1982,7 @@
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>251371</v>
+        <v>251477</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
@@ -1988,33 +1990,33 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="D21" t="n">
-        <v>0</v>
+        <v>468.734375</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>2025-05-07 12:07:45</t>
+          <t>2025-05-08 14:42:25</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>2025-05-07 12:26:45</t>
+          <t>2025-05-09 07:14:25</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>2025-05-07 12:26:45</t>
+          <t>2025-05-09 07:14:25</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>2025-05-07 12:26:45</t>
+          <t>2025-05-12 07:03:09</t>
         </is>
       </c>
       <c r="I21" t="n">
-        <v>0</v>
+        <v>29999</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
@@ -2023,19 +2025,17 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L21" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M21" t="n">
-        <v>70</v>
-      </c>
-      <c r="N21" t="inlineStr">
-        <is>
-          <t>39666 (esterno)</t>
-        </is>
+        <v>76</v>
+      </c>
+      <c r="N21" t="n">
+        <v>39760</v>
       </c>
       <c r="O21" t="inlineStr">
         <is>
@@ -2043,23 +2043,23 @@
         </is>
       </c>
       <c r="P21" t="n">
-        <v>39666</v>
+        <v>39760</v>
       </c>
       <c r="Q21" t="inlineStr">
         <is>
-          <t>2025-04-24 00:00:00</t>
+          <t>2025-04-28 00:00:00</t>
         </is>
       </c>
       <c r="R21" s="1" t="n">
-        <v>-13.51857638888889</v>
+        <v>-5.293858506944445</v>
       </c>
       <c r="S21" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>251396</v>
+        <v>251782</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
@@ -2067,33 +2067,33 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D22" t="n">
-        <v>35.34375</v>
+        <v>188.640625</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>2025-05-07 12:26:45</t>
+          <t>2025-05-12 07:03:09</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>2025-05-07 12:45:45</t>
+          <t>2025-05-12 07:18:09</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>2025-05-07 12:45:45</t>
+          <t>2025-05-12 07:18:09</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>2025-05-07 13:21:05</t>
+          <t>2025-05-12 10:26:47</t>
         </is>
       </c>
       <c r="I22" t="n">
-        <v>2262</v>
+        <v>12073</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
@@ -2102,17 +2102,17 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L22" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="M22" t="n">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="N22" t="n">
-        <v>39749</v>
+        <v>39754</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
@@ -2120,57 +2120,57 @@
         </is>
       </c>
       <c r="P22" t="n">
-        <v>39749</v>
+        <v>39754</v>
       </c>
       <c r="Q22" t="inlineStr">
         <is>
-          <t>2025-05-02 00:00:00</t>
+          <t>2025-05-16 00:00:00</t>
         </is>
       </c>
       <c r="R22" s="1" t="n">
-        <v>-0.5563151041666666</v>
+        <v>-3.435275607638889</v>
       </c>
       <c r="S22" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>251548</v>
+        <v>251371</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="D23" t="n">
-        <v>206.90625</v>
+        <v>0</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>2025-05-07 13:21:05</t>
+          <t>2025-05-08 07:00:00</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>2025-05-07 13:40:05</t>
+          <t>2025-05-08 07:34:00</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>2025-05-07 13:40:05</t>
+          <t>2025-05-08 07:34:00</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>2025-05-08 09:07:00</t>
+          <t>2025-05-08 07:34:00</t>
         </is>
       </c>
       <c r="I23" t="n">
-        <v>13242</v>
+        <v>0</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
@@ -2188,8 +2188,10 @@
       <c r="M23" t="n">
         <v>70</v>
       </c>
-      <c r="N23" t="n">
-        <v>39749</v>
+      <c r="N23" t="inlineStr">
+        <is>
+          <t>39666 (esterno)</t>
+        </is>
       </c>
       <c r="O23" t="inlineStr">
         <is>
@@ -2197,15 +2199,15 @@
         </is>
       </c>
       <c r="P23" t="n">
-        <v>39749</v>
+        <v>39666</v>
       </c>
       <c r="Q23" t="inlineStr">
         <is>
-          <t>2025-05-06 00:00:00</t>
+          <t>2025-04-24 00:00:00</t>
         </is>
       </c>
       <c r="R23" s="1" t="n">
-        <v>-1.379861111111111</v>
+        <v>-14.31527777777778</v>
       </c>
       <c r="S23" t="n">
         <v>7</v>
@@ -2213,41 +2215,41 @@
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>250923</v>
+        <v>251547</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="D24" t="n">
-        <v>109.46875</v>
+        <v>184.9154929577465</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>2025-05-08 09:07:00</t>
+          <t>2025-05-08 07:34:00</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>2025-05-08 09:39:00</t>
+          <t>2025-05-08 07:49:00</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>2025-05-08 09:39:00</t>
+          <t>2025-05-08 07:49:00</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>2025-05-08 11:28:28</t>
+          <t>2025-05-08 10:53:54</t>
         </is>
       </c>
       <c r="I24" t="n">
-        <v>7006</v>
+        <v>13129</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
@@ -2256,14 +2258,14 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L24" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M24" t="n">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="N24" t="n">
         <v>39749</v>
@@ -2278,53 +2280,53 @@
       </c>
       <c r="Q24" t="inlineStr">
         <is>
-          <t>2025-04-07 00:00:00</t>
+          <t>2025-05-06 00:00:00</t>
         </is>
       </c>
       <c r="R24" s="1" t="n">
-        <v>-1.478103298611111</v>
+        <v>-1.454107981215278</v>
       </c>
       <c r="S24" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>251477</v>
+        <v>250759</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="D25" t="n">
-        <v>468.734375</v>
+        <v>118.2816901408451</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>2025-05-08 11:28:28</t>
+          <t>2025-05-08 10:53:54</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>2025-05-08 11:47:28</t>
+          <t>2025-05-08 11:23:54</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>2025-05-08 11:47:28</t>
+          <t>2025-05-08 11:23:54</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>2025-05-09 11:36:12</t>
+          <t>2025-05-08 13:22:11</t>
         </is>
       </c>
       <c r="I25" t="n">
-        <v>29999</v>
+        <v>8398</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
@@ -2333,17 +2335,17 @@
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12</t>
         </is>
       </c>
       <c r="L25" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M25" t="n">
         <v>76</v>
       </c>
       <c r="N25" t="n">
-        <v>39760</v>
+        <v>39747</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
@@ -2351,15 +2353,15 @@
         </is>
       </c>
       <c r="P25" t="n">
-        <v>39760</v>
+        <v>39747</v>
       </c>
       <c r="Q25" t="inlineStr">
         <is>
-          <t>2025-04-28 00:00:00</t>
+          <t>2025-03-13 00:00:00</t>
         </is>
       </c>
       <c r="R25" s="1" t="n">
-        <v>-2.483474392361111</v>
+        <v>-0.5570813771527778</v>
       </c>
       <c r="S25" t="n">
         <v>1</v>
@@ -2367,7 +2369,7 @@
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>251456</v>
+        <v>251416</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
@@ -2375,10 +2377,10 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="D26" t="n">
-        <v>183.6530612244898</v>
+        <v>229.0204081632653</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
@@ -2387,21 +2389,21 @@
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>2025-05-08 07:40:00</t>
+          <t>2025-05-08 07:35:00</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>2025-05-08 07:40:00</t>
+          <t>2025-05-08 07:35:00</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>2025-05-08 10:43:39</t>
+          <t>2025-05-08 11:24:01</t>
         </is>
       </c>
       <c r="I26" t="n">
-        <v>8999</v>
+        <v>11222</v>
       </c>
       <c r="J26" t="inlineStr">
         <is>
@@ -2414,71 +2416,69 @@
         </is>
       </c>
       <c r="L26" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M26" t="n">
         <v>70</v>
       </c>
       <c r="N26" t="n">
-        <v>39746</v>
-      </c>
-      <c r="O26" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
+        <v>39755</v>
+      </c>
+      <c r="O26" t="n">
+        <v>0</v>
       </c>
       <c r="P26" t="n">
-        <v>39746</v>
+        <v>0</v>
       </c>
       <c r="Q26" t="inlineStr">
         <is>
-          <t>2025-05-09 00:00:00</t>
+          <t>2025-04-23 00:00:00</t>
         </is>
       </c>
       <c r="R26" s="1" t="n">
-        <v>-2.446981292511574</v>
+        <v>0</v>
       </c>
       <c r="S26" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>251416</v>
+        <v>251651</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>R3</t>
+          <t>BIMEC 4</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="D27" t="n">
-        <v>229.0204081632653</v>
+        <v>767.7049180327868</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>2025-05-08 10:43:39</t>
+          <t>2025-05-09 07:00:00</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>2025-05-08 11:23:39</t>
+          <t>2025-05-09 07:29:00</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>2025-05-08 11:23:39</t>
+          <t>2025-05-09 07:29:00</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>2025-05-09 07:12:40</t>
+          <t>2025-05-12 12:16:42</t>
         </is>
       </c>
       <c r="I27" t="n">
-        <v>11222</v>
+        <v>46830</v>
       </c>
       <c r="J27" t="inlineStr">
         <is>
@@ -2487,14 +2487,14 @@
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L27" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="M27" t="n">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="N27" t="n">
         <v>39755</v>
@@ -2507,14 +2507,14 @@
       </c>
       <c r="Q27" t="inlineStr">
         <is>
-          <t>2025-04-23 00:00:00</t>
+          <t>2025-05-12 00:00:00</t>
         </is>
       </c>
       <c r="R27" s="1" t="n">
         <v>0</v>
       </c>
       <c r="S27" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Continua a rompersi solo LS3
</commit_message>
<xml_diff>
--- a/PS-VRP/Dati_output/insert_inter.xlsx
+++ b/PS-VRP/Dati_output/insert_inter.xlsx
@@ -519,7 +519,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>R12</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -530,22 +530,22 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2025-05-08 12:00:00</t>
+          <t>2025-05-08 07:00:00</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2025-05-08 12:19:00</t>
+          <t>2025-05-08 07:19:00</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>2025-05-08 12:19:00</t>
+          <t>2025-05-08 07:19:00</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>2025-05-08 12:19:00</t>
+          <t>2025-05-08 07:19:00</t>
         </is>
       </c>
       <c r="I2" t="n">
@@ -584,7 +584,7 @@
         </is>
       </c>
       <c r="R2" s="1" t="n">
-        <v>-0.5131944444444444</v>
+        <v>-0.3048611111111111</v>
       </c>
       <c r="S2" t="n">
         <v>1</v>
@@ -592,41 +592,41 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>251227</v>
+        <v>251455</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>R12</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="D3" t="n">
-        <v>0</v>
+        <v>74.6056338028169</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2025-05-08 12:19:00</t>
+          <t>2025-05-08 07:19:00</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2025-05-08 12:34:00</t>
+          <t>2025-05-08 07:49:00</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>2025-05-08 12:34:00</t>
+          <t>2025-05-08 07:49:00</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>2025-05-08 12:34:00</t>
+          <t>2025-05-08 09:03:36</t>
         </is>
       </c>
       <c r="I3" t="n">
-        <v>0</v>
+        <v>5297</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
@@ -635,17 +635,17 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L3" t="n">
         <v>4</v>
       </c>
       <c r="M3" t="n">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="N3" t="n">
-        <v>39746</v>
+        <v>39749</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
@@ -653,57 +653,57 @@
         </is>
       </c>
       <c r="P3" t="n">
-        <v>39746</v>
+        <v>39749</v>
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>2025-05-05 00:00:00</t>
+          <t>2025-04-15 00:00:00</t>
         </is>
       </c>
       <c r="R3" s="1" t="n">
-        <v>-2.523611111111111</v>
+        <v>-1.377503912361111</v>
       </c>
       <c r="S3" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>250923</v>
+        <v>251547</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>R12</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D4" t="n">
-        <v>98.67605633802818</v>
+        <v>184.9154929577465</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2025-05-08 12:34:00</t>
+          <t>2025-05-08 09:03:36</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>2025-05-08 12:51:00</t>
+          <t>2025-05-08 09:18:36</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>2025-05-08 12:51:00</t>
+          <t>2025-05-08 09:18:36</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>2025-05-08 14:29:40</t>
+          <t>2025-05-08 12:23:31</t>
         </is>
       </c>
       <c r="I4" t="n">
-        <v>7006</v>
+        <v>13129</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
@@ -712,14 +712,14 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L4" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M4" t="n">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="N4" t="n">
         <v>39749</v>
@@ -734,53 +734,53 @@
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>2025-04-07 00:00:00</t>
+          <t>2025-05-06 00:00:00</t>
         </is>
       </c>
       <c r="R4" s="1" t="n">
-        <v>-1.603941705787037</v>
+        <v>-1.516334115810185</v>
       </c>
       <c r="S4" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>250894</v>
+        <v>250759</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>R12</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="D5" t="n">
-        <v>623.4084507042254</v>
+        <v>118.2816901408451</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2025-05-08 14:29:40</t>
+          <t>2025-05-08 12:23:31</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>2025-05-08 14:44:40</t>
+          <t>2025-05-08 12:53:31</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>2025-05-08 14:44:40</t>
+          <t>2025-05-08 12:53:31</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>2025-05-12 09:08:05</t>
+          <t>2025-05-08 14:51:48</t>
         </is>
       </c>
       <c r="I5" t="n">
-        <v>44262</v>
+        <v>8398</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
@@ -789,152 +789,150 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12</t>
         </is>
       </c>
       <c r="L5" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M5" t="n">
         <v>76</v>
       </c>
       <c r="N5" t="n">
-        <v>39755</v>
-      </c>
-      <c r="O5" t="n">
-        <v>0</v>
+        <v>39747</v>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
       </c>
       <c r="P5" t="n">
-        <v>0</v>
+        <v>39747</v>
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>2025-05-05 00:00:00</t>
+          <t>2025-03-13 00:00:00</t>
         </is>
       </c>
       <c r="R5" s="1" t="n">
-        <v>0</v>
+        <v>-0.6193075117361111</v>
       </c>
       <c r="S5" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>251706</v>
+        <v>250894</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>T3</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C6" t="n">
+        <v>17</v>
+      </c>
+      <c r="D6" t="n">
+        <v>623.4084507042254</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>2025-05-08 14:51:48</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>2025-05-09 07:08:48</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>2025-05-09 07:08:48</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>2025-05-12 09:32:12</t>
+        </is>
+      </c>
+      <c r="I6" t="n">
+        <v>44262</v>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>bobina</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R6 ;R9</t>
+        </is>
+      </c>
+      <c r="L6" t="n">
+        <v>5</v>
+      </c>
+      <c r="M6" t="n">
+        <v>76</v>
+      </c>
+      <c r="N6" t="n">
+        <v>39755</v>
+      </c>
+      <c r="O6" t="n">
         <v>0</v>
       </c>
-      <c r="D6" t="n">
-        <v>50.79365079365079</v>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>2025-05-12 07:00:00</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>2025-05-12 07:00:00</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>2025-05-12 07:00:00</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>2025-05-12 07:50:47</t>
-        </is>
-      </c>
-      <c r="I6" t="n">
-        <v>3200</v>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>foglio</t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>T3</t>
-        </is>
-      </c>
-      <c r="L6" t="n">
+      <c r="P6" t="n">
         <v>0</v>
       </c>
-      <c r="M6" t="n">
-        <v>0</v>
-      </c>
-      <c r="N6" t="inlineStr">
-        <is>
-          <t>39764 (esterno)</t>
-        </is>
-      </c>
-      <c r="O6" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="P6" t="n">
-        <v>39764</v>
-      </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>2025-05-14 00:00:00</t>
+          <t>2025-05-05 00:00:00</t>
         </is>
       </c>
       <c r="R6" s="1" t="n">
         <v>0</v>
       </c>
       <c r="S6" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>251164</v>
+        <v>251227</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>57</v>
+        <v>34</v>
       </c>
       <c r="D7" t="n">
-        <v>140.8450704225352</v>
+        <v>0</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2025-05-09 07:00:00</t>
+          <t>2025-05-07 07:00:00</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>2025-05-09 07:57:00</t>
+          <t>2025-05-07 07:34:00</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>2025-05-09 07:57:00</t>
+          <t>2025-05-07 07:34:00</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>2025-05-09 10:17:50</t>
+          <t>2025-05-07 07:34:00</t>
         </is>
       </c>
       <c r="I7" t="n">
-        <v>10000</v>
+        <v>0</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
@@ -943,17 +941,17 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
         </is>
       </c>
       <c r="L7" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="M7" t="n">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="N7" t="n">
-        <v>39749</v>
+        <v>39746</v>
       </c>
       <c r="O7" t="inlineStr">
         <is>
@@ -961,57 +959,57 @@
         </is>
       </c>
       <c r="P7" t="n">
-        <v>39749</v>
+        <v>39746</v>
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>2025-04-22 00:00:00</t>
+          <t>2025-05-05 00:00:00</t>
         </is>
       </c>
       <c r="R7" s="1" t="n">
-        <v>-2.429059076678241</v>
+        <v>-1.315277777777778</v>
       </c>
       <c r="S7" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>251050</v>
+        <v>251164</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>195</v>
+        <v>34</v>
       </c>
       <c r="D8" t="n">
-        <v>0</v>
+        <v>156.25</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2025-05-09 10:17:50</t>
+          <t>2025-05-07 07:34:00</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>2025-05-09 13:32:50</t>
+          <t>2025-05-07 08:08:00</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>2025-05-09 13:32:50</t>
+          <t>2025-05-07 08:08:00</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>2025-05-09 13:32:50</t>
+          <t>2025-05-07 10:44:15</t>
         </is>
       </c>
       <c r="I8" t="n">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
@@ -1020,17 +1018,17 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L8" t="n">
-        <v>38</v>
+        <v>6</v>
       </c>
       <c r="M8" t="n">
         <v>70</v>
       </c>
       <c r="N8" t="n">
-        <v>39747</v>
+        <v>39749</v>
       </c>
       <c r="O8" t="inlineStr">
         <is>
@@ -1038,57 +1036,57 @@
         </is>
       </c>
       <c r="P8" t="n">
-        <v>39747</v>
+        <v>39749</v>
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>2025-04-16 00:00:00</t>
+          <t>2025-04-22 00:00:00</t>
         </is>
       </c>
       <c r="R8" s="1" t="n">
-        <v>-1.564475743344907</v>
+        <v>-0.4473958333333333</v>
       </c>
       <c r="S8" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>251054</v>
+        <v>251391</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="D9" t="n">
-        <v>0</v>
+        <v>91.640625</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>2025-05-09 13:32:50</t>
+          <t>2025-05-07 10:44:15</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>2025-05-09 14:07:50</t>
+          <t>2025-05-07 11:01:15</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>2025-05-09 14:07:50</t>
+          <t>2025-05-07 11:01:15</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>2025-05-09 14:07:50</t>
+          <t>2025-05-07 12:32:53</t>
         </is>
       </c>
       <c r="I9" t="n">
-        <v>0</v>
+        <v>5865</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
@@ -1097,17 +1095,17 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L9" t="n">
-        <v>38</v>
+        <v>5</v>
       </c>
       <c r="M9" t="n">
         <v>70</v>
       </c>
       <c r="N9" t="n">
-        <v>39747</v>
+        <v>39749</v>
       </c>
       <c r="O9" t="inlineStr">
         <is>
@@ -1115,57 +1113,57 @@
         </is>
       </c>
       <c r="P9" t="n">
-        <v>39747</v>
+        <v>39749</v>
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>2025-04-16 00:00:00</t>
+          <t>2025-04-23 00:00:00</t>
         </is>
       </c>
       <c r="R9" s="1" t="n">
-        <v>-1.588781298900463</v>
+        <v>-0.5228407118055556</v>
       </c>
       <c r="S9" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>251081</v>
+        <v>251395</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>125</v>
+        <v>17</v>
       </c>
       <c r="D10" t="n">
-        <v>42.42253521126761</v>
+        <v>35.34375</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2025-05-09 14:07:50</t>
+          <t>2025-05-07 12:32:53</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>2025-05-12 08:12:50</t>
+          <t>2025-05-07 12:49:53</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>2025-05-12 08:12:50</t>
+          <t>2025-05-07 12:49:53</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>2025-05-12 08:55:16</t>
+          <t>2025-05-07 13:25:14</t>
         </is>
       </c>
       <c r="I10" t="n">
-        <v>3012</v>
+        <v>2262</v>
       </c>
       <c r="J10" t="inlineStr">
         <is>
@@ -1174,19 +1172,17 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L10" t="n">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="M10" t="n">
         <v>70</v>
       </c>
-      <c r="N10" t="inlineStr">
-        <is>
-          <t>39750 (esterno)</t>
-        </is>
+      <c r="N10" t="n">
+        <v>39749</v>
       </c>
       <c r="O10" t="inlineStr">
         <is>
@@ -1194,7 +1190,7 @@
         </is>
       </c>
       <c r="P10" t="n">
-        <v>39750</v>
+        <v>39749</v>
       </c>
       <c r="Q10" t="inlineStr">
         <is>
@@ -1202,49 +1198,49 @@
         </is>
       </c>
       <c r="R10" s="1" t="n">
-        <v>-19.37171361502315</v>
+        <v>-0.5591905381944444</v>
       </c>
       <c r="S10" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>251284</v>
+        <v>251371</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>CASON</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>40.5</v>
+        <v>19</v>
       </c>
       <c r="D11" t="n">
-        <v>297.0909090909091</v>
+        <v>0</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>2025-05-09 07:00:00</t>
+          <t>2025-05-07 13:25:14</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>2025-05-09 07:40:30</t>
+          <t>2025-05-07 13:44:14</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>2025-05-09 07:40:30</t>
+          <t>2025-05-07 13:44:14</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>2025-05-09 12:37:35</t>
+          <t>2025-05-07 13:44:14</t>
         </is>
       </c>
       <c r="I11" t="n">
-        <v>16340</v>
+        <v>0</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
@@ -1253,17 +1249,19 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>CASON ;R6</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L11" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="M11" t="n">
         <v>70</v>
       </c>
-      <c r="N11" t="n">
-        <v>39747</v>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>39666 (esterno)</t>
+        </is>
       </c>
       <c r="O11" t="inlineStr">
         <is>
@@ -1271,57 +1269,57 @@
         </is>
       </c>
       <c r="P11" t="n">
-        <v>39747</v>
+        <v>39666</v>
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>2025-05-12 00:00:00</t>
+          <t>2025-04-24 00:00:00</t>
         </is>
       </c>
       <c r="R11" s="1" t="n">
-        <v>-1.526104797974537</v>
+        <v>-13.57238498263889</v>
       </c>
       <c r="S11" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>251229</v>
+        <v>251396</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>40</v>
+        <v>19</v>
       </c>
       <c r="D12" t="n">
-        <v>307.1967213114754</v>
+        <v>35.34375</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>2025-05-08 07:00:00</t>
+          <t>2025-05-07 13:44:14</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>2025-05-08 07:40:00</t>
+          <t>2025-05-07 14:03:14</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>2025-05-08 07:40:00</t>
+          <t>2025-05-07 14:03:14</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>2025-05-08 12:47:11</t>
+          <t>2025-05-07 14:38:34</t>
         </is>
       </c>
       <c r="I12" t="n">
-        <v>18739</v>
+        <v>2262</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
@@ -1330,7 +1328,7 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L12" t="n">
@@ -1339,10 +1337,8 @@
       <c r="M12" t="n">
         <v>70</v>
       </c>
-      <c r="N12" t="inlineStr">
-        <is>
-          <t>39723 (esterno)</t>
-        </is>
+      <c r="N12" t="n">
+        <v>39749</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
@@ -1350,23 +1346,23 @@
         </is>
       </c>
       <c r="P12" t="n">
-        <v>39723</v>
+        <v>39749</v>
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>2025-05-15 00:00:00</t>
+          <t>2025-05-02 00:00:00</t>
         </is>
       </c>
       <c r="R12" s="1" t="n">
-        <v>0</v>
+        <v>-0.6101236979166667</v>
       </c>
       <c r="S12" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>251456</v>
+        <v>251548</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
@@ -1374,33 +1370,33 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D13" t="n">
-        <v>140.609375</v>
+        <v>206.90625</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>2025-05-07 07:00:00</t>
+          <t>2025-05-07 14:38:34</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>2025-05-07 07:17:00</t>
+          <t>2025-05-07 14:57:34</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>2025-05-07 07:17:00</t>
+          <t>2025-05-07 14:57:34</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>2025-05-07 09:37:36</t>
+          <t>2025-05-08 10:24:29</t>
         </is>
       </c>
       <c r="I13" t="n">
-        <v>8999</v>
+        <v>13242</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
@@ -1413,13 +1409,13 @@
         </is>
       </c>
       <c r="L13" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M13" t="n">
         <v>70</v>
       </c>
       <c r="N13" t="n">
-        <v>39746</v>
+        <v>39749</v>
       </c>
       <c r="O13" t="inlineStr">
         <is>
@@ -1427,23 +1423,23 @@
         </is>
       </c>
       <c r="P13" t="n">
-        <v>39746</v>
+        <v>39749</v>
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>2025-05-09 00:00:00</t>
+          <t>2025-05-06 00:00:00</t>
         </is>
       </c>
       <c r="R13" s="1" t="n">
-        <v>-1.401117621527778</v>
+        <v>-1.433669704861111</v>
       </c>
       <c r="S13" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>251742</v>
+        <v>250923</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
@@ -1451,33 +1447,33 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="D14" t="n">
-        <v>128.53125</v>
+        <v>109.46875</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>2025-05-07 09:37:36</t>
+          <t>2025-05-08 10:24:29</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>2025-05-07 09:54:36</t>
+          <t>2025-05-08 10:56:29</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>2025-05-07 09:54:36</t>
+          <t>2025-05-08 10:56:29</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>2025-05-07 12:03:08</t>
+          <t>2025-05-08 12:45:57</t>
         </is>
       </c>
       <c r="I14" t="n">
-        <v>8226</v>
+        <v>7006</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
@@ -1486,14 +1482,14 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
         </is>
       </c>
       <c r="L14" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M14" t="n">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="N14" t="n">
         <v>39749</v>
@@ -1508,19 +1504,19 @@
       </c>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>2025-05-15 00:00:00</t>
+          <t>2025-04-07 00:00:00</t>
         </is>
       </c>
       <c r="R14" s="1" t="n">
-        <v>-0.5021809895833333</v>
+        <v>-1.531911892361111</v>
       </c>
       <c r="S14" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>251455</v>
+        <v>251477</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
@@ -1528,33 +1524,33 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D15" t="n">
-        <v>82.765625</v>
+        <v>468.734375</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>2025-05-07 12:03:08</t>
+          <t>2025-05-08 12:45:57</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>2025-05-07 12:18:08</t>
+          <t>2025-05-08 13:04:57</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>2025-05-07 12:18:08</t>
+          <t>2025-05-08 13:04:57</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>2025-05-07 13:40:54</t>
+          <t>2025-05-09 12:53:41</t>
         </is>
       </c>
       <c r="I15" t="n">
-        <v>5297</v>
+        <v>29999</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
@@ -1563,17 +1559,17 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L15" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M15" t="n">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="N15" t="n">
-        <v>39749</v>
+        <v>39760</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
@@ -1581,76 +1577,78 @@
         </is>
       </c>
       <c r="P15" t="n">
-        <v>39749</v>
+        <v>39760</v>
       </c>
       <c r="Q15" t="inlineStr">
         <is>
-          <t>2025-04-15 00:00:00</t>
+          <t>2025-04-28 00:00:00</t>
         </is>
       </c>
       <c r="R15" s="1" t="n">
-        <v>-0.5700737847222223</v>
+        <v>-2.537282986111111</v>
       </c>
       <c r="S15" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>251840</v>
+        <v>251706</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>T3</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="D16" t="n">
-        <v>89.28125</v>
+        <v>50.79365079365079</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>2025-05-07 13:40:54</t>
+          <t>2025-05-12 07:00:00</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>2025-05-07 13:57:54</t>
+          <t>2025-05-12 07:00:00</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>2025-05-07 13:57:54</t>
+          <t>2025-05-12 07:00:00</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>2025-05-08 07:27:11</t>
+          <t>2025-05-12 07:50:47</t>
         </is>
       </c>
       <c r="I16" t="n">
-        <v>5714</v>
+        <v>3200</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>bobina</t>
+          <t>foglio</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>T3</t>
         </is>
       </c>
       <c r="L16" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="M16" t="n">
-        <v>70</v>
-      </c>
-      <c r="N16" t="n">
-        <v>39758</v>
+        <v>0</v>
+      </c>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>39764 (esterno)</t>
+        </is>
       </c>
       <c r="O16" t="inlineStr">
         <is>
@@ -1658,57 +1656,57 @@
         </is>
       </c>
       <c r="P16" t="n">
-        <v>39758</v>
+        <v>39764</v>
       </c>
       <c r="Q16" t="inlineStr">
         <is>
-          <t>2025-05-09 00:00:00</t>
+          <t>2025-05-14 00:00:00</t>
         </is>
       </c>
       <c r="R16" s="1" t="n">
-        <v>-0.310546875</v>
+        <v>0</v>
       </c>
       <c r="S16" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>251391</v>
+        <v>251050</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>15</v>
+        <v>217</v>
       </c>
       <c r="D17" t="n">
-        <v>91.640625</v>
+        <v>0</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>2025-05-08 07:27:11</t>
+          <t>2025-05-09 07:00:00</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>2025-05-08 07:42:11</t>
+          <t>2025-05-09 10:37:00</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>2025-05-08 07:42:11</t>
+          <t>2025-05-09 10:37:00</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>2025-05-08 09:13:49</t>
+          <t>2025-05-09 10:37:00</t>
         </is>
       </c>
       <c r="I17" t="n">
-        <v>5865</v>
+        <v>0</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
@@ -1717,17 +1715,17 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="L17" t="n">
-        <v>5</v>
+        <v>38</v>
       </c>
       <c r="M17" t="n">
         <v>70</v>
       </c>
       <c r="N17" t="n">
-        <v>39749</v>
+        <v>39747</v>
       </c>
       <c r="O17" t="inlineStr">
         <is>
@@ -1735,57 +1733,57 @@
         </is>
       </c>
       <c r="P17" t="n">
-        <v>39749</v>
+        <v>39747</v>
       </c>
       <c r="Q17" t="inlineStr">
         <is>
-          <t>2025-04-23 00:00:00</t>
+          <t>2025-04-16 00:00:00</t>
         </is>
       </c>
       <c r="R17" s="1" t="n">
-        <v>-1.384602864583333</v>
+        <v>-1.442361111111111</v>
       </c>
       <c r="S17" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>251395</v>
+        <v>251054</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="D18" t="n">
-        <v>35.34375</v>
+        <v>0</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>2025-05-08 09:13:49</t>
+          <t>2025-05-09 10:37:00</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>2025-05-08 09:30:49</t>
+          <t>2025-05-09 11:12:00</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>2025-05-08 09:30:49</t>
+          <t>2025-05-09 11:12:00</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>2025-05-08 10:06:10</t>
+          <t>2025-05-09 11:12:00</t>
         </is>
       </c>
       <c r="I18" t="n">
-        <v>2262</v>
+        <v>0</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
@@ -1794,17 +1792,17 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="L18" t="n">
-        <v>6</v>
+        <v>38</v>
       </c>
       <c r="M18" t="n">
         <v>70</v>
       </c>
       <c r="N18" t="n">
-        <v>39749</v>
+        <v>39747</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
@@ -1812,57 +1810,57 @@
         </is>
       </c>
       <c r="P18" t="n">
-        <v>39749</v>
+        <v>39747</v>
       </c>
       <c r="Q18" t="inlineStr">
         <is>
-          <t>2025-04-23 00:00:00</t>
+          <t>2025-04-16 00:00:00</t>
         </is>
       </c>
       <c r="R18" s="1" t="n">
-        <v>-1.420952690972222</v>
+        <v>-1.466666666666667</v>
       </c>
       <c r="S18" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>251396</v>
+        <v>251081</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>15</v>
+        <v>125</v>
       </c>
       <c r="D19" t="n">
-        <v>35.34375</v>
+        <v>42.42253521126761</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>2025-05-08 10:06:10</t>
+          <t>2025-05-09 11:12:00</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>2025-05-08 10:21:10</t>
+          <t>2025-05-09 13:17:00</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>2025-05-08 10:21:10</t>
+          <t>2025-05-09 13:17:00</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>2025-05-08 10:56:30</t>
+          <t>2025-05-09 13:59:25</t>
         </is>
       </c>
       <c r="I19" t="n">
-        <v>2262</v>
+        <v>3012</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
@@ -1871,17 +1869,19 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="L19" t="n">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="M19" t="n">
         <v>70</v>
       </c>
-      <c r="N19" t="n">
-        <v>39749</v>
+      <c r="N19" t="inlineStr">
+        <is>
+          <t>39750 (esterno)</t>
+        </is>
       </c>
       <c r="O19" t="inlineStr">
         <is>
@@ -1889,57 +1889,57 @@
         </is>
       </c>
       <c r="P19" t="n">
-        <v>39749</v>
+        <v>39750</v>
       </c>
       <c r="Q19" t="inlineStr">
         <is>
-          <t>2025-05-02 00:00:00</t>
+          <t>2025-04-23 00:00:00</t>
         </is>
       </c>
       <c r="R19" s="1" t="n">
-        <v>-1.455913628472222</v>
+        <v>-16.58293231612268</v>
       </c>
       <c r="S19" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>251548</v>
+        <v>251742</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>R10</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="D20" t="n">
-        <v>206.90625</v>
+        <v>134.8524590163935</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>2025-05-08 10:56:30</t>
+          <t>2025-05-08 07:00:00</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>2025-05-08 11:15:30</t>
+          <t>2025-05-08 07:30:00</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>2025-05-08 11:15:30</t>
+          <t>2025-05-08 07:30:00</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>2025-05-08 14:42:25</t>
+          <t>2025-05-08 09:44:51</t>
         </is>
       </c>
       <c r="I20" t="n">
-        <v>13242</v>
+        <v>8226</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
@@ -1970,11 +1970,11 @@
       </c>
       <c r="Q20" t="inlineStr">
         <is>
-          <t>2025-05-06 00:00:00</t>
+          <t>2025-05-15 00:00:00</t>
         </is>
       </c>
       <c r="R20" s="1" t="n">
-        <v>-1.61279296875</v>
+        <v>-1.406147540983796</v>
       </c>
       <c r="S20" t="n">
         <v>7</v>
@@ -1982,41 +1982,41 @@
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>251477</v>
+        <v>251840</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>R10</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="D21" t="n">
-        <v>468.734375</v>
+        <v>93.67213114754098</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>2025-05-08 14:42:25</t>
+          <t>2025-05-08 09:44:51</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>2025-05-09 07:14:25</t>
+          <t>2025-05-08 10:09:51</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>2025-05-09 07:14:25</t>
+          <t>2025-05-08 10:09:51</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>2025-05-12 07:03:09</t>
+          <t>2025-05-08 11:43:31</t>
         </is>
       </c>
       <c r="I21" t="n">
-        <v>29999</v>
+        <v>5714</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
@@ -2025,17 +2025,17 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L21" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="M21" t="n">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="N21" t="n">
-        <v>39760</v>
+        <v>39758</v>
       </c>
       <c r="O21" t="inlineStr">
         <is>
@@ -2043,15 +2043,15 @@
         </is>
       </c>
       <c r="P21" t="n">
-        <v>39760</v>
+        <v>39758</v>
       </c>
       <c r="Q21" t="inlineStr">
         <is>
-          <t>2025-04-28 00:00:00</t>
+          <t>2025-05-09 00:00:00</t>
         </is>
       </c>
       <c r="R21" s="1" t="n">
-        <v>-5.293858506944445</v>
+        <v>-0.4885587431712963</v>
       </c>
       <c r="S21" t="n">
         <v>1</v>
@@ -2059,41 +2059,41 @@
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>251782</v>
+        <v>251229</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>R10</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="D22" t="n">
-        <v>188.640625</v>
+        <v>307.1967213114754</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>2025-05-12 07:03:09</t>
+          <t>2025-05-08 11:43:31</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>2025-05-12 07:18:09</t>
+          <t>2025-05-08 12:08:31</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>2025-05-12 07:18:09</t>
+          <t>2025-05-08 12:08:31</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>2025-05-12 10:26:47</t>
+          <t>2025-05-09 09:15:43</t>
         </is>
       </c>
       <c r="I22" t="n">
-        <v>12073</v>
+        <v>18739</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
@@ -2102,17 +2102,19 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R9</t>
         </is>
       </c>
       <c r="L22" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="M22" t="n">
-        <v>76</v>
-      </c>
-      <c r="N22" t="n">
-        <v>39754</v>
+        <v>70</v>
+      </c>
+      <c r="N22" t="inlineStr">
+        <is>
+          <t>39723 (esterno)</t>
+        </is>
       </c>
       <c r="O22" t="inlineStr">
         <is>
@@ -2120,15 +2122,15 @@
         </is>
       </c>
       <c r="P22" t="n">
-        <v>39754</v>
+        <v>39723</v>
       </c>
       <c r="Q22" t="inlineStr">
         <is>
-          <t>2025-05-16 00:00:00</t>
+          <t>2025-05-15 00:00:00</t>
         </is>
       </c>
       <c r="R22" s="1" t="n">
-        <v>-3.435275607638889</v>
+        <v>0</v>
       </c>
       <c r="S22" t="n">
         <v>1</v>
@@ -2136,120 +2138,116 @@
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>251371</v>
+        <v>251651</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>BIMEC 5</t>
+          <t>BIMEC 4</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D23" t="n">
+        <v>767.7049180327868</v>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>2025-05-09 07:00:00</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>2025-05-09 07:29:00</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>2025-05-09 07:29:00</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>2025-05-12 12:16:42</t>
+        </is>
+      </c>
+      <c r="I23" t="n">
+        <v>46830</v>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>bobina</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R6 ;R9</t>
+        </is>
+      </c>
+      <c r="L23" t="n">
+        <v>5</v>
+      </c>
+      <c r="M23" t="n">
+        <v>76</v>
+      </c>
+      <c r="N23" t="n">
+        <v>39755</v>
+      </c>
+      <c r="O23" t="n">
         <v>0</v>
       </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>2025-05-08 07:00:00</t>
-        </is>
-      </c>
-      <c r="F23" t="inlineStr">
-        <is>
-          <t>2025-05-08 07:34:00</t>
-        </is>
-      </c>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>2025-05-08 07:34:00</t>
-        </is>
-      </c>
-      <c r="H23" t="inlineStr">
-        <is>
-          <t>2025-05-08 07:34:00</t>
-        </is>
-      </c>
-      <c r="I23" t="n">
+      <c r="P23" t="n">
         <v>0</v>
       </c>
-      <c r="J23" t="inlineStr">
-        <is>
-          <t>bobina</t>
-        </is>
-      </c>
-      <c r="K23" t="inlineStr">
-        <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
-        </is>
-      </c>
-      <c r="L23" t="n">
+      <c r="Q23" t="inlineStr">
+        <is>
+          <t>2025-05-12 00:00:00</t>
+        </is>
+      </c>
+      <c r="R23" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="S23" t="n">
         <v>4</v>
-      </c>
-      <c r="M23" t="n">
-        <v>70</v>
-      </c>
-      <c r="N23" t="inlineStr">
-        <is>
-          <t>39666 (esterno)</t>
-        </is>
-      </c>
-      <c r="O23" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="P23" t="n">
-        <v>39666</v>
-      </c>
-      <c r="Q23" t="inlineStr">
-        <is>
-          <t>2025-04-24 00:00:00</t>
-        </is>
-      </c>
-      <c r="R23" s="1" t="n">
-        <v>-14.31527777777778</v>
-      </c>
-      <c r="S23" t="n">
-        <v>7</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>251547</v>
+        <v>251456</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>BIMEC 5</t>
+          <t>R3</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="D24" t="n">
-        <v>184.9154929577465</v>
+        <v>183.6530612244898</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>2025-05-08 07:34:00</t>
+          <t>2025-05-08 07:00:00</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>2025-05-08 07:49:00</t>
+          <t>2025-05-08 07:40:00</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>2025-05-08 07:49:00</t>
+          <t>2025-05-08 07:40:00</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>2025-05-08 10:53:54</t>
+          <t>2025-05-08 10:43:39</t>
         </is>
       </c>
       <c r="I24" t="n">
-        <v>13129</v>
+        <v>8999</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
@@ -2262,13 +2260,13 @@
         </is>
       </c>
       <c r="L24" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M24" t="n">
         <v>70</v>
       </c>
       <c r="N24" t="n">
-        <v>39749</v>
+        <v>39746</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
@@ -2276,57 +2274,57 @@
         </is>
       </c>
       <c r="P24" t="n">
-        <v>39749</v>
+        <v>39746</v>
       </c>
       <c r="Q24" t="inlineStr">
         <is>
-          <t>2025-05-06 00:00:00</t>
+          <t>2025-05-09 00:00:00</t>
         </is>
       </c>
       <c r="R24" s="1" t="n">
-        <v>-1.454107981215278</v>
+        <v>-2.446981292511574</v>
       </c>
       <c r="S24" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>250759</v>
+        <v>251416</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>BIMEC 5</t>
+          <t>R3</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="D25" t="n">
-        <v>118.2816901408451</v>
+        <v>229.0204081632653</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>2025-05-08 10:53:54</t>
+          <t>2025-05-08 10:43:39</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>2025-05-08 11:23:54</t>
+          <t>2025-05-08 11:23:39</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>2025-05-08 11:23:54</t>
+          <t>2025-05-08 11:23:39</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>2025-05-08 13:22:11</t>
+          <t>2025-05-09 07:12:40</t>
         </is>
       </c>
       <c r="I25" t="n">
-        <v>8398</v>
+        <v>11222</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
@@ -2335,75 +2333,73 @@
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L25" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="M25" t="n">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="N25" t="n">
-        <v>39747</v>
-      </c>
-      <c r="O25" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
+        <v>39755</v>
+      </c>
+      <c r="O25" t="n">
+        <v>0</v>
       </c>
       <c r="P25" t="n">
-        <v>39747</v>
+        <v>0</v>
       </c>
       <c r="Q25" t="inlineStr">
         <is>
-          <t>2025-03-13 00:00:00</t>
+          <t>2025-04-23 00:00:00</t>
         </is>
       </c>
       <c r="R25" s="1" t="n">
-        <v>-0.5570813771527778</v>
+        <v>0</v>
       </c>
       <c r="S25" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>251416</v>
+        <v>251782</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>R3</t>
+          <t>R12</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="D26" t="n">
-        <v>229.0204081632653</v>
+        <v>170.0422535211268</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>2025-05-08 07:00:00</t>
+          <t>2025-05-08 12:00:00</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>2025-05-08 07:35:00</t>
+          <t>2025-05-08 12:17:00</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>2025-05-08 07:35:00</t>
+          <t>2025-05-08 12:17:00</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>2025-05-08 11:24:01</t>
+          <t>2025-05-09 07:07:02</t>
         </is>
       </c>
       <c r="I26" t="n">
-        <v>11222</v>
+        <v>12073</v>
       </c>
       <c r="J26" t="inlineStr">
         <is>
@@ -2412,50 +2408,52 @@
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L26" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M26" t="n">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="N26" t="n">
-        <v>39755</v>
-      </c>
-      <c r="O26" t="n">
-        <v>0</v>
+        <v>39754</v>
+      </c>
+      <c r="O26" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
       </c>
       <c r="P26" t="n">
-        <v>0</v>
+        <v>39754</v>
       </c>
       <c r="Q26" t="inlineStr">
         <is>
-          <t>2025-04-23 00:00:00</t>
+          <t>2025-05-16 00:00:00</t>
         </is>
       </c>
       <c r="R26" s="1" t="n">
-        <v>0</v>
+        <v>-0.2965571204976852</v>
       </c>
       <c r="S26" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>251651</v>
+        <v>251284</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>BIMEC 4</t>
+          <t>CASON</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>29</v>
+        <v>40.5</v>
       </c>
       <c r="D27" t="n">
-        <v>767.7049180327868</v>
+        <v>297.0909090909091</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
@@ -2464,21 +2462,21 @@
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>2025-05-09 07:29:00</t>
+          <t>2025-05-09 07:40:30</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>2025-05-09 07:29:00</t>
+          <t>2025-05-09 07:40:30</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>2025-05-12 12:16:42</t>
+          <t>2025-05-09 12:37:35</t>
         </is>
       </c>
       <c r="I27" t="n">
-        <v>46830</v>
+        <v>16340</v>
       </c>
       <c r="J27" t="inlineStr">
         <is>
@@ -2487,23 +2485,25 @@
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R6 ;R9</t>
+          <t>CASON ;R6</t>
         </is>
       </c>
       <c r="L27" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="M27" t="n">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="N27" t="n">
-        <v>39755</v>
-      </c>
-      <c r="O27" t="n">
-        <v>0</v>
+        <v>39747</v>
+      </c>
+      <c r="O27" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
       </c>
       <c r="P27" t="n">
-        <v>0</v>
+        <v>39747</v>
       </c>
       <c r="Q27" t="inlineStr">
         <is>
@@ -2511,10 +2511,10 @@
         </is>
       </c>
       <c r="R27" s="1" t="n">
-        <v>0</v>
+        <v>-1.526104797974537</v>
       </c>
       <c r="S27" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Dovrebbe andare tutto bene
</commit_message>
<xml_diff>
--- a/PS-VRP/Dati_output/insert_inter.xlsx
+++ b/PS-VRP/Dati_output/insert_inter.xlsx
@@ -515,41 +515,41 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>251229</v>
+        <v>251164</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="D2" t="n">
-        <v>307.1967213114754</v>
+        <v>156.25</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2025-05-08 07:00:00</t>
+          <t>2025-05-07 07:00:00</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2025-05-08 07:40:00</t>
+          <t>2025-05-07 07:23:00</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>2025-05-08 07:40:00</t>
+          <t>2025-05-07 07:23:00</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>2025-05-08 12:47:11</t>
+          <t>2025-05-07 09:59:15</t>
         </is>
       </c>
       <c r="I2" t="n">
-        <v>18739</v>
+        <v>10000</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
@@ -558,7 +558,7 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L2" t="n">
@@ -567,10 +567,8 @@
       <c r="M2" t="n">
         <v>70</v>
       </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>39723 (esterno)</t>
-        </is>
+      <c r="N2" t="n">
+        <v>39749</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
@@ -578,57 +576,57 @@
         </is>
       </c>
       <c r="P2" t="n">
-        <v>39723</v>
+        <v>39749</v>
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>2025-05-15 00:00:00</t>
+          <t>2025-04-22 00:00:00</t>
         </is>
       </c>
       <c r="R2" s="1" t="n">
-        <v>0</v>
+        <v>-0.4161458333333333</v>
       </c>
       <c r="S2" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>251164</v>
+        <v>251371</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>57</v>
+        <v>19</v>
       </c>
       <c r="D3" t="n">
-        <v>140.8450704225352</v>
+        <v>0</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2025-05-09 07:00:00</t>
+          <t>2025-05-07 09:59:15</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2025-05-09 07:57:00</t>
+          <t>2025-05-07 10:18:15</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>2025-05-09 07:57:00</t>
+          <t>2025-05-07 10:18:15</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>2025-05-09 10:17:50</t>
+          <t>2025-05-07 10:18:15</t>
         </is>
       </c>
       <c r="I3" t="n">
-        <v>10000</v>
+        <v>0</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
@@ -641,13 +639,15 @@
         </is>
       </c>
       <c r="L3" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="M3" t="n">
         <v>70</v>
       </c>
-      <c r="N3" t="n">
-        <v>39749</v>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>39666 (esterno)</t>
+        </is>
       </c>
       <c r="O3" t="inlineStr">
         <is>
@@ -655,57 +655,57 @@
         </is>
       </c>
       <c r="P3" t="n">
-        <v>39749</v>
+        <v>39666</v>
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>2025-04-22 00:00:00</t>
+          <t>2025-04-24 00:00:00</t>
         </is>
       </c>
       <c r="R3" s="1" t="n">
-        <v>-2.429059076678241</v>
+        <v>-13.42934027777778</v>
       </c>
       <c r="S3" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>251050</v>
+        <v>251391</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>195</v>
+        <v>17</v>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>91.640625</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2025-05-09 10:17:50</t>
+          <t>2025-05-07 10:18:15</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>2025-05-09 13:32:50</t>
+          <t>2025-05-07 10:35:15</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>2025-05-09 13:32:50</t>
+          <t>2025-05-07 10:35:15</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>2025-05-09 13:32:50</t>
+          <t>2025-05-07 12:06:53</t>
         </is>
       </c>
       <c r="I4" t="n">
-        <v>0</v>
+        <v>5865</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
@@ -714,17 +714,17 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L4" t="n">
-        <v>38</v>
+        <v>5</v>
       </c>
       <c r="M4" t="n">
         <v>70</v>
       </c>
       <c r="N4" t="n">
-        <v>39747</v>
+        <v>39749</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
@@ -732,57 +732,57 @@
         </is>
       </c>
       <c r="P4" t="n">
-        <v>39747</v>
+        <v>39749</v>
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>2025-04-16 00:00:00</t>
+          <t>2025-04-23 00:00:00</t>
         </is>
       </c>
       <c r="R4" s="1" t="n">
-        <v>-1.564475743344907</v>
+        <v>-0.50478515625</v>
       </c>
       <c r="S4" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>251054</v>
+        <v>251395</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="D5" t="n">
-        <v>0</v>
+        <v>35.34375</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2025-05-09 13:32:50</t>
+          <t>2025-05-07 12:06:53</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>2025-05-09 14:07:50</t>
+          <t>2025-05-07 12:23:53</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>2025-05-09 14:07:50</t>
+          <t>2025-05-07 12:23:53</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>2025-05-09 14:07:50</t>
+          <t>2025-05-07 12:59:14</t>
         </is>
       </c>
       <c r="I5" t="n">
-        <v>0</v>
+        <v>2262</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
@@ -791,17 +791,17 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L5" t="n">
-        <v>38</v>
+        <v>6</v>
       </c>
       <c r="M5" t="n">
         <v>70</v>
       </c>
       <c r="N5" t="n">
-        <v>39747</v>
+        <v>39749</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
@@ -809,57 +809,57 @@
         </is>
       </c>
       <c r="P5" t="n">
-        <v>39747</v>
+        <v>39749</v>
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>2025-04-16 00:00:00</t>
+          <t>2025-04-23 00:00:00</t>
         </is>
       </c>
       <c r="R5" s="1" t="n">
-        <v>-1.588781298900463</v>
+        <v>-0.5411349826388889</v>
       </c>
       <c r="S5" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>251081</v>
+        <v>251396</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>125</v>
+        <v>15</v>
       </c>
       <c r="D6" t="n">
-        <v>42.42253521126761</v>
+        <v>35.34375</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2025-05-09 14:07:50</t>
+          <t>2025-05-07 12:59:14</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2025-05-12 08:12:50</t>
+          <t>2025-05-07 13:14:14</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>2025-05-12 08:12:50</t>
+          <t>2025-05-07 13:14:14</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>2025-05-12 08:55:16</t>
+          <t>2025-05-07 13:49:34</t>
         </is>
       </c>
       <c r="I6" t="n">
-        <v>3012</v>
+        <v>2262</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
@@ -868,19 +868,17 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L6" t="n">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="M6" t="n">
         <v>70</v>
       </c>
-      <c r="N6" t="inlineStr">
-        <is>
-          <t>39750 (esterno)</t>
-        </is>
+      <c r="N6" t="n">
+        <v>39749</v>
       </c>
       <c r="O6" t="inlineStr">
         <is>
@@ -888,57 +886,57 @@
         </is>
       </c>
       <c r="P6" t="n">
-        <v>39750</v>
+        <v>39749</v>
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>2025-04-23 00:00:00</t>
+          <t>2025-05-02 00:00:00</t>
         </is>
       </c>
       <c r="R6" s="1" t="n">
-        <v>-19.37171361502315</v>
+        <v>-0.5760959201388889</v>
       </c>
       <c r="S6" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>251416</v>
+        <v>251548</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>R3</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="D7" t="n">
-        <v>229.0204081632653</v>
+        <v>206.90625</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2025-05-08 07:00:00</t>
+          <t>2025-05-07 13:49:34</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>2025-05-08 07:35:00</t>
+          <t>2025-05-07 14:08:34</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>2025-05-08 07:35:00</t>
+          <t>2025-05-07 14:08:34</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>2025-05-08 11:24:01</t>
+          <t>2025-05-08 09:35:29</t>
         </is>
       </c>
       <c r="I7" t="n">
-        <v>11222</v>
+        <v>13242</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
@@ -951,69 +949,71 @@
         </is>
       </c>
       <c r="L7" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M7" t="n">
         <v>70</v>
       </c>
       <c r="N7" t="n">
-        <v>39755</v>
-      </c>
-      <c r="O7" t="n">
-        <v>0</v>
+        <v>39749</v>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
       </c>
       <c r="P7" t="n">
-        <v>0</v>
+        <v>39749</v>
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>2025-04-23 00:00:00</t>
+          <t>2025-05-06 00:00:00</t>
         </is>
       </c>
       <c r="R7" s="1" t="n">
-        <v>0</v>
+        <v>-1.399641927083333</v>
       </c>
       <c r="S7" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>251227</v>
+        <v>251477</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>R12</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="D8" t="n">
-        <v>0</v>
+        <v>468.734375</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2025-05-08 12:00:00</t>
+          <t>2025-05-08 09:35:29</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>2025-05-08 12:19:00</t>
+          <t>2025-05-08 10:07:29</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>2025-05-08 12:19:00</t>
+          <t>2025-05-08 10:07:29</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>2025-05-08 12:19:00</t>
+          <t>2025-05-09 09:56:13</t>
         </is>
       </c>
       <c r="I8" t="n">
-        <v>0</v>
+        <v>29999</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
@@ -1022,17 +1022,17 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L8" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M8" t="n">
         <v>76</v>
       </c>
       <c r="N8" t="n">
-        <v>39746</v>
+        <v>39760</v>
       </c>
       <c r="O8" t="inlineStr">
         <is>
@@ -1040,15 +1040,15 @@
         </is>
       </c>
       <c r="P8" t="n">
-        <v>39746</v>
+        <v>39760</v>
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>2025-05-05 00:00:00</t>
+          <t>2025-04-28 00:00:00</t>
         </is>
       </c>
       <c r="R8" s="1" t="n">
-        <v>-2.513194444444444</v>
+        <v>-2.414040798611111</v>
       </c>
       <c r="S8" t="n">
         <v>1</v>
@@ -1060,33 +1060,33 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>BIMEC 5</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D9" t="n">
-        <v>170.0422535211268</v>
+        <v>188.640625</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>2025-05-08 07:00:00</t>
+          <t>2025-05-09 09:56:13</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>2025-05-08 07:17:00</t>
+          <t>2025-05-09 10:11:13</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>2025-05-08 07:17:00</t>
+          <t>2025-05-09 10:11:13</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>2025-05-08 10:07:02</t>
+          <t>2025-05-09 13:19:51</t>
         </is>
       </c>
       <c r="I9" t="n">
@@ -1125,7 +1125,7 @@
         </is>
       </c>
       <c r="R9" s="1" t="n">
-        <v>0</v>
+        <v>-0.5554578993055556</v>
       </c>
       <c r="S9" t="n">
         <v>1</v>
@@ -1133,86 +1133,82 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>251371</v>
+        <v>251651</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>BIMEC 5</t>
+          <t>BIMEC 4</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D10" t="n">
+        <v>767.7049180327868</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>2025-05-09 07:00:00</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>2025-05-09 07:29:00</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>2025-05-09 07:29:00</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>2025-05-12 12:16:42</t>
+        </is>
+      </c>
+      <c r="I10" t="n">
+        <v>46830</v>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>bobina</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R6 ;R9</t>
+        </is>
+      </c>
+      <c r="L10" t="n">
+        <v>5</v>
+      </c>
+      <c r="M10" t="n">
+        <v>76</v>
+      </c>
+      <c r="N10" t="n">
+        <v>39755</v>
+      </c>
+      <c r="O10" t="n">
         <v>0</v>
       </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>2025-05-08 10:07:02</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>2025-05-08 10:39:02</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>2025-05-08 10:39:02</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>2025-05-08 10:39:02</t>
-        </is>
-      </c>
-      <c r="I10" t="n">
+      <c r="P10" t="n">
         <v>0</v>
       </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>bobina</t>
-        </is>
-      </c>
-      <c r="K10" t="inlineStr">
-        <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
-        </is>
-      </c>
-      <c r="L10" t="n">
+      <c r="Q10" t="inlineStr">
+        <is>
+          <t>2025-05-12 00:00:00</t>
+        </is>
+      </c>
+      <c r="R10" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="S10" t="n">
         <v>4</v>
-      </c>
-      <c r="M10" t="n">
-        <v>70</v>
-      </c>
-      <c r="N10" t="inlineStr">
-        <is>
-          <t>39666 (esterno)</t>
-        </is>
-      </c>
-      <c r="O10" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="P10" t="n">
-        <v>39666</v>
-      </c>
-      <c r="Q10" t="inlineStr">
-        <is>
-          <t>2025-04-24 00:00:00</t>
-        </is>
-      </c>
-      <c r="R10" s="1" t="n">
-        <v>-14.44377934271991</v>
-      </c>
-      <c r="S10" t="n">
-        <v>7</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>251456</v>
+        <v>251225</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
@@ -1220,33 +1216,33 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D11" t="n">
-        <v>126.7464788732394</v>
+        <v>0</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>2025-05-08 10:39:02</t>
+          <t>2025-05-08 07:00:00</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>2025-05-08 10:56:02</t>
+          <t>2025-05-08 07:19:00</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>2025-05-08 10:56:02</t>
+          <t>2025-05-08 07:19:00</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>2025-05-08 13:02:47</t>
+          <t>2025-05-08 07:19:00</t>
         </is>
       </c>
       <c r="I11" t="n">
-        <v>8999</v>
+        <v>0</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
@@ -1255,17 +1251,17 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
         </is>
       </c>
       <c r="L11" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M11" t="n">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="N11" t="n">
-        <v>39746</v>
+        <v>39747</v>
       </c>
       <c r="O11" t="inlineStr">
         <is>
@@ -1273,15 +1269,15 @@
         </is>
       </c>
       <c r="P11" t="n">
-        <v>39746</v>
+        <v>39747</v>
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>2025-05-09 00:00:00</t>
+          <t>2025-04-30 00:00:00</t>
         </is>
       </c>
       <c r="R11" s="1" t="n">
-        <v>-2.543603286388889</v>
+        <v>-0.3048611111111111</v>
       </c>
       <c r="S11" t="n">
         <v>1</v>
@@ -1289,7 +1285,7 @@
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>251840</v>
+        <v>251456</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
@@ -1297,33 +1293,33 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="D12" t="n">
-        <v>80.47887323943662</v>
+        <v>126.7464788732394</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>2025-05-08 13:02:47</t>
+          <t>2025-05-08 07:19:00</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>2025-05-08 13:21:47</t>
+          <t>2025-05-08 07:51:00</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>2025-05-08 13:21:47</t>
+          <t>2025-05-08 07:51:00</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>2025-05-08 14:42:16</t>
+          <t>2025-05-08 09:57:44</t>
         </is>
       </c>
       <c r="I12" t="n">
-        <v>5714</v>
+        <v>8999</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
@@ -1336,13 +1332,13 @@
         </is>
       </c>
       <c r="L12" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="M12" t="n">
         <v>70</v>
       </c>
       <c r="N12" t="n">
-        <v>39758</v>
+        <v>39746</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
@@ -1350,7 +1346,7 @@
         </is>
       </c>
       <c r="P12" t="n">
-        <v>39758</v>
+        <v>39746</v>
       </c>
       <c r="Q12" t="inlineStr">
         <is>
@@ -1358,7 +1354,7 @@
         </is>
       </c>
       <c r="R12" s="1" t="n">
-        <v>-0.6126858372453704</v>
+        <v>-2.415101721435185</v>
       </c>
       <c r="S12" t="n">
         <v>1</v>
@@ -1366,7 +1362,7 @@
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>251547</v>
+        <v>251455</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
@@ -1377,30 +1373,30 @@
         <v>17</v>
       </c>
       <c r="D13" t="n">
-        <v>184.9154929577465</v>
+        <v>74.6056338028169</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>2025-05-08 14:42:16</t>
+          <t>2025-05-08 09:57:44</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>2025-05-08 14:59:16</t>
+          <t>2025-05-08 10:14:44</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>2025-05-08 14:59:16</t>
+          <t>2025-05-08 10:14:44</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>2025-05-09 10:04:10</t>
+          <t>2025-05-08 11:29:21</t>
         </is>
       </c>
       <c r="I13" t="n">
-        <v>13129</v>
+        <v>5297</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
@@ -1431,11 +1427,11 @@
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>2025-05-06 00:00:00</t>
+          <t>2025-04-15 00:00:00</t>
         </is>
       </c>
       <c r="R13" s="1" t="n">
-        <v>-2.419571596238426</v>
+        <v>-1.478716744918982</v>
       </c>
       <c r="S13" t="n">
         <v>7</v>
@@ -1443,7 +1439,7 @@
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>250759</v>
+        <v>251547</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
@@ -1451,33 +1447,33 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="D14" t="n">
-        <v>118.2816901408451</v>
+        <v>184.9154929577465</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>2025-05-09 10:04:10</t>
+          <t>2025-05-08 11:29:21</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>2025-05-09 10:34:10</t>
+          <t>2025-05-08 11:44:21</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>2025-05-09 10:34:10</t>
+          <t>2025-05-08 11:44:21</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>2025-05-09 12:32:27</t>
+          <t>2025-05-08 14:49:16</t>
         </is>
       </c>
       <c r="I14" t="n">
-        <v>8398</v>
+        <v>13129</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
@@ -1486,17 +1482,17 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L14" t="n">
         <v>4</v>
       </c>
       <c r="M14" t="n">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="N14" t="n">
-        <v>39747</v>
+        <v>39749</v>
       </c>
       <c r="O14" t="inlineStr">
         <is>
@@ -1504,23 +1500,23 @@
         </is>
       </c>
       <c r="P14" t="n">
-        <v>39747</v>
+        <v>39749</v>
       </c>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>2025-03-13 00:00:00</t>
+          <t>2025-05-06 00:00:00</t>
         </is>
       </c>
       <c r="R14" s="1" t="n">
-        <v>-1.522544992175926</v>
+        <v>-1.617546948356481</v>
       </c>
       <c r="S14" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>250894</v>
+        <v>250759</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
@@ -1528,33 +1524,33 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="D15" t="n">
-        <v>623.4084507042254</v>
+        <v>118.2816901408451</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>2025-05-09 12:32:27</t>
+          <t>2025-05-08 14:49:16</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>2025-05-09 12:49:27</t>
+          <t>2025-05-09 07:19:16</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>2025-05-09 12:49:27</t>
+          <t>2025-05-09 07:19:16</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>2025-05-13 07:12:52</t>
+          <t>2025-05-09 09:17:32</t>
         </is>
       </c>
       <c r="I15" t="n">
-        <v>44262</v>
+        <v>8398</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
@@ -1563,73 +1559,75 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12</t>
         </is>
       </c>
       <c r="L15" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M15" t="n">
         <v>76</v>
       </c>
       <c r="N15" t="n">
-        <v>39755</v>
-      </c>
-      <c r="O15" t="n">
-        <v>0</v>
+        <v>39747</v>
+      </c>
+      <c r="O15" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
       </c>
       <c r="P15" t="n">
-        <v>0</v>
+        <v>39747</v>
       </c>
       <c r="Q15" t="inlineStr">
         <is>
-          <t>2025-05-05 00:00:00</t>
+          <t>2025-03-13 00:00:00</t>
         </is>
       </c>
       <c r="R15" s="1" t="n">
-        <v>-0.3006064162731482</v>
+        <v>-1.387187010949074</v>
       </c>
       <c r="S15" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>251651</v>
+        <v>250894</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>BIMEC 4</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="D16" t="n">
-        <v>767.7049180327868</v>
+        <v>623.4084507042254</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>2025-05-09 07:00:00</t>
+          <t>2025-05-09 09:17:32</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>2025-05-09 07:29:00</t>
+          <t>2025-05-09 09:34:32</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>2025-05-09 07:29:00</t>
+          <t>2025-05-09 09:34:32</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>2025-05-12 12:16:42</t>
+          <t>2025-05-12 11:57:57</t>
         </is>
       </c>
       <c r="I16" t="n">
-        <v>46830</v>
+        <v>44262</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
@@ -1658,7 +1656,7 @@
       </c>
       <c r="Q16" t="inlineStr">
         <is>
-          <t>2025-05-12 00:00:00</t>
+          <t>2025-05-05 00:00:00</t>
         </is>
       </c>
       <c r="R16" s="1" t="n">
@@ -1751,33 +1749,33 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>R10</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="D18" t="n">
-        <v>128.53125</v>
+        <v>134.8524590163935</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>2025-05-07 07:00:00</t>
+          <t>2025-05-08 07:00:00</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>2025-05-07 07:19:00</t>
+          <t>2025-05-08 07:30:00</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>2025-05-07 07:19:00</t>
+          <t>2025-05-08 07:30:00</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>2025-05-07 09:27:31</t>
+          <t>2025-05-08 09:44:51</t>
         </is>
       </c>
       <c r="I18" t="n">
@@ -1816,7 +1814,7 @@
         </is>
       </c>
       <c r="R18" s="1" t="n">
-        <v>-0.3941189236111111</v>
+        <v>-1.406147540983796</v>
       </c>
       <c r="S18" t="n">
         <v>7</v>
@@ -1824,41 +1822,41 @@
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>251455</v>
+        <v>251840</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>R10</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="D19" t="n">
-        <v>82.765625</v>
+        <v>93.67213114754098</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>2025-05-07 09:27:31</t>
+          <t>2025-05-08 09:44:51</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>2025-05-07 09:42:31</t>
+          <t>2025-05-08 10:09:51</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>2025-05-07 09:42:31</t>
+          <t>2025-05-08 10:09:51</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>2025-05-07 11:05:17</t>
+          <t>2025-05-08 11:43:31</t>
         </is>
       </c>
       <c r="I19" t="n">
-        <v>5297</v>
+        <v>5714</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
@@ -1871,13 +1869,13 @@
         </is>
       </c>
       <c r="L19" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M19" t="n">
         <v>70</v>
       </c>
       <c r="N19" t="n">
-        <v>39749</v>
+        <v>39758</v>
       </c>
       <c r="O19" t="inlineStr">
         <is>
@@ -1885,57 +1883,57 @@
         </is>
       </c>
       <c r="P19" t="n">
-        <v>39749</v>
+        <v>39758</v>
       </c>
       <c r="Q19" t="inlineStr">
         <is>
-          <t>2025-04-15 00:00:00</t>
+          <t>2025-05-09 00:00:00</t>
         </is>
       </c>
       <c r="R19" s="1" t="n">
-        <v>-0.46201171875</v>
+        <v>-0.4885587431712963</v>
       </c>
       <c r="S19" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>251391</v>
+        <v>251229</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>R10</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="D20" t="n">
-        <v>91.640625</v>
+        <v>307.1967213114754</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>2025-05-07 11:05:17</t>
+          <t>2025-05-08 11:43:31</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>2025-05-07 11:22:17</t>
+          <t>2025-05-08 12:08:31</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>2025-05-07 11:22:17</t>
+          <t>2025-05-08 12:08:31</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>2025-05-07 12:53:56</t>
+          <t>2025-05-09 09:15:43</t>
         </is>
       </c>
       <c r="I20" t="n">
-        <v>5865</v>
+        <v>18739</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
@@ -1944,17 +1942,19 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R9</t>
         </is>
       </c>
       <c r="L20" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M20" t="n">
         <v>70</v>
       </c>
-      <c r="N20" t="n">
-        <v>39749</v>
+      <c r="N20" t="inlineStr">
+        <is>
+          <t>39723 (esterno)</t>
+        </is>
       </c>
       <c r="O20" t="inlineStr">
         <is>
@@ -1962,57 +1962,57 @@
         </is>
       </c>
       <c r="P20" t="n">
-        <v>39749</v>
+        <v>39723</v>
       </c>
       <c r="Q20" t="inlineStr">
         <is>
-          <t>2025-04-23 00:00:00</t>
+          <t>2025-05-15 00:00:00</t>
         </is>
       </c>
       <c r="R20" s="1" t="n">
-        <v>-0.5374565972222223</v>
+        <v>0</v>
       </c>
       <c r="S20" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>251395</v>
+        <v>250923</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>R12</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D21" t="n">
-        <v>35.34375</v>
+        <v>98.67605633802818</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>2025-05-07 12:53:56</t>
+          <t>2025-05-08 12:00:00</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>2025-05-07 13:10:56</t>
+          <t>2025-05-08 12:21:00</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>2025-05-07 13:10:56</t>
+          <t>2025-05-08 12:21:00</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>2025-05-07 13:46:16</t>
+          <t>2025-05-08 13:59:40</t>
         </is>
       </c>
       <c r="I21" t="n">
-        <v>2262</v>
+        <v>7006</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
@@ -2021,14 +2021,14 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
         </is>
       </c>
       <c r="L21" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="M21" t="n">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="N21" t="n">
         <v>39749</v>
@@ -2043,53 +2043,53 @@
       </c>
       <c r="Q21" t="inlineStr">
         <is>
-          <t>2025-04-23 00:00:00</t>
+          <t>2025-04-07 00:00:00</t>
         </is>
       </c>
       <c r="R21" s="1" t="n">
-        <v>-0.5738064236111111</v>
+        <v>-1.583108372453704</v>
       </c>
       <c r="S21" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>251396</v>
+        <v>251227</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>R12</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D22" t="n">
-        <v>35.34375</v>
+        <v>0</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>2025-05-07 13:46:16</t>
+          <t>2025-05-08 13:59:40</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>2025-05-07 14:01:16</t>
+          <t>2025-05-08 14:16:40</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>2025-05-07 14:01:16</t>
+          <t>2025-05-08 14:16:40</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>2025-05-07 14:36:37</t>
+          <t>2025-05-08 14:16:40</t>
         </is>
       </c>
       <c r="I22" t="n">
-        <v>2262</v>
+        <v>0</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
@@ -2098,17 +2098,17 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
         </is>
       </c>
       <c r="L22" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="M22" t="n">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="N22" t="n">
-        <v>39749</v>
+        <v>39746</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
@@ -2116,57 +2116,57 @@
         </is>
       </c>
       <c r="P22" t="n">
-        <v>39749</v>
+        <v>39746</v>
       </c>
       <c r="Q22" t="inlineStr">
         <is>
-          <t>2025-05-02 00:00:00</t>
+          <t>2025-05-05 00:00:00</t>
         </is>
       </c>
       <c r="R22" s="1" t="n">
-        <v>-0.6087673611111111</v>
+        <v>-2.594913928009259</v>
       </c>
       <c r="S22" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>251548</v>
+        <v>251416</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>R3</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="D23" t="n">
-        <v>206.90625</v>
+        <v>229.0204081632653</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>2025-05-07 14:36:37</t>
+          <t>2025-05-08 07:00:00</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>2025-05-07 14:55:37</t>
+          <t>2025-05-08 07:35:00</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>2025-05-07 14:55:37</t>
+          <t>2025-05-08 07:35:00</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>2025-05-08 10:22:31</t>
+          <t>2025-05-08 11:24:01</t>
         </is>
       </c>
       <c r="I23" t="n">
-        <v>13242</v>
+        <v>11222</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
@@ -2179,67 +2179,65 @@
         </is>
       </c>
       <c r="L23" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="M23" t="n">
         <v>70</v>
       </c>
       <c r="N23" t="n">
-        <v>39749</v>
-      </c>
-      <c r="O23" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
+        <v>39755</v>
+      </c>
+      <c r="O23" t="n">
+        <v>0</v>
       </c>
       <c r="P23" t="n">
-        <v>39749</v>
+        <v>0</v>
       </c>
       <c r="Q23" t="inlineStr">
         <is>
-          <t>2025-05-06 00:00:00</t>
+          <t>2025-04-23 00:00:00</t>
         </is>
       </c>
       <c r="R23" s="1" t="n">
-        <v>-1.432313368055556</v>
+        <v>0</v>
       </c>
       <c r="S23" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>251225</v>
+        <v>251050</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>30</v>
+        <v>217</v>
       </c>
       <c r="D24" t="n">
         <v>0</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>2025-05-08 10:22:31</t>
+          <t>2025-05-09 07:00:00</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>2025-05-08 10:52:31</t>
+          <t>2025-05-09 10:37:00</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>2025-05-08 10:52:31</t>
+          <t>2025-05-09 10:37:00</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>2025-05-08 10:52:31</t>
+          <t>2025-05-09 10:37:00</t>
         </is>
       </c>
       <c r="I24" t="n">
@@ -2252,14 +2250,14 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="L24" t="n">
-        <v>4</v>
+        <v>38</v>
       </c>
       <c r="M24" t="n">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="N24" t="n">
         <v>39747</v>
@@ -2274,53 +2272,53 @@
       </c>
       <c r="Q24" t="inlineStr">
         <is>
-          <t>2025-04-30 00:00:00</t>
+          <t>2025-04-16 00:00:00</t>
         </is>
       </c>
       <c r="R24" s="1" t="n">
-        <v>-0.4531467013888889</v>
+        <v>-1.442361111111111</v>
       </c>
       <c r="S24" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>250923</v>
+        <v>251054</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="D25" t="n">
-        <v>109.46875</v>
+        <v>0</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>2025-05-08 10:52:31</t>
+          <t>2025-05-09 10:37:00</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>2025-05-08 11:09:31</t>
+          <t>2025-05-09 11:12:00</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>2025-05-08 11:09:31</t>
+          <t>2025-05-09 11:12:00</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>2025-05-08 12:59:00</t>
+          <t>2025-05-09 11:12:00</t>
         </is>
       </c>
       <c r="I25" t="n">
-        <v>7006</v>
+        <v>0</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
@@ -2329,17 +2327,17 @@
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="L25" t="n">
-        <v>5</v>
+        <v>38</v>
       </c>
       <c r="M25" t="n">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="N25" t="n">
-        <v>39749</v>
+        <v>39747</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
@@ -2347,15 +2345,15 @@
         </is>
       </c>
       <c r="P25" t="n">
-        <v>39749</v>
+        <v>39747</v>
       </c>
       <c r="Q25" t="inlineStr">
         <is>
-          <t>2025-04-07 00:00:00</t>
+          <t>2025-04-16 00:00:00</t>
         </is>
       </c>
       <c r="R25" s="1" t="n">
-        <v>-1.540972222222222</v>
+        <v>-1.466666666666667</v>
       </c>
       <c r="S25" t="n">
         <v>2</v>
@@ -2363,41 +2361,41 @@
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>251477</v>
+        <v>251081</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>19</v>
+        <v>125</v>
       </c>
       <c r="D26" t="n">
-        <v>468.734375</v>
+        <v>42.42253521126761</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>2025-05-08 12:59:00</t>
+          <t>2025-05-09 11:12:00</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>2025-05-08 13:18:00</t>
+          <t>2025-05-09 13:17:00</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>2025-05-08 13:18:00</t>
+          <t>2025-05-09 13:17:00</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>2025-05-09 13:06:44</t>
+          <t>2025-05-09 13:59:25</t>
         </is>
       </c>
       <c r="I26" t="n">
-        <v>29999</v>
+        <v>3012</v>
       </c>
       <c r="J26" t="inlineStr">
         <is>
@@ -2406,17 +2404,19 @@
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R6 ;R9</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="L26" t="n">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="M26" t="n">
-        <v>76</v>
-      </c>
-      <c r="N26" t="n">
-        <v>39760</v>
+        <v>70</v>
+      </c>
+      <c r="N26" t="inlineStr">
+        <is>
+          <t>39750 (esterno)</t>
+        </is>
       </c>
       <c r="O26" t="inlineStr">
         <is>
@@ -2424,18 +2424,18 @@
         </is>
       </c>
       <c r="P26" t="n">
-        <v>39760</v>
+        <v>39750</v>
       </c>
       <c r="Q26" t="inlineStr">
         <is>
-          <t>2025-04-28 00:00:00</t>
+          <t>2025-04-23 00:00:00</t>
         </is>
       </c>
       <c r="R26" s="1" t="n">
-        <v>-2.546343315972222</v>
+        <v>-16.58293231612268</v>
       </c>
       <c r="S26" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27">

</xml_diff>